<commit_message>
Enhance scraper logging and add detailed environment status checks
Co-authored-by: jongpard <jongpard@gmail.com>
</commit_message>
<xml_diff>
--- a/oliveyoung_rankings_2025-08-13.xlsx
+++ b/oliveyoung_rankings_2025-08-13.xlsx
@@ -489,7 +489,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:10.822534+09:00</t>
+          <t>2025-08-13T01:55:53.253319+09:00</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:10.854632+09:00</t>
+          <t>2025-08-13T01:55:53.285291+09:00</t>
         </is>
       </c>
     </row>
@@ -545,7 +545,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:10.901398+09:00</t>
+          <t>2025-08-13T01:55:53.321593+09:00</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:10.930760+09:00</t>
+          <t>2025-08-13T01:55:53.367439+09:00</t>
         </is>
       </c>
     </row>
@@ -601,7 +601,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:10.979894+09:00</t>
+          <t>2025-08-13T01:55:53.423481+09:00</t>
         </is>
       </c>
     </row>
@@ -629,7 +629,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.030958+09:00</t>
+          <t>2025-08-13T01:55:53.482434+09:00</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.083207+09:00</t>
+          <t>2025-08-13T01:55:53.538615+09:00</t>
         </is>
       </c>
     </row>
@@ -685,7 +685,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.131467+09:00</t>
+          <t>2025-08-13T01:55:53.585426+09:00</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.179670+09:00</t>
+          <t>2025-08-13T01:55:53.625601+09:00</t>
         </is>
       </c>
     </row>
@@ -741,7 +741,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.224019+09:00</t>
+          <t>2025-08-13T01:55:53.665736+09:00</t>
         </is>
       </c>
     </row>
@@ -769,7 +769,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.244839+09:00</t>
+          <t>2025-08-13T01:55:53.685832+09:00</t>
         </is>
       </c>
     </row>
@@ -797,7 +797,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.261970+09:00</t>
+          <t>2025-08-13T01:55:53.704012+09:00</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.278010+09:00</t>
+          <t>2025-08-13T01:55:53.722664+09:00</t>
         </is>
       </c>
     </row>
@@ -853,7 +853,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.302384+09:00</t>
+          <t>2025-08-13T01:55:53.767675+09:00</t>
         </is>
       </c>
     </row>
@@ -881,7 +881,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.352059+09:00</t>
+          <t>2025-08-13T01:55:53.823886+09:00</t>
         </is>
       </c>
     </row>
@@ -909,7 +909,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.397604+09:00</t>
+          <t>2025-08-13T01:55:53.859082+09:00</t>
         </is>
       </c>
     </row>
@@ -937,7 +937,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.432431+09:00</t>
+          <t>2025-08-13T01:55:53.909603+09:00</t>
         </is>
       </c>
     </row>
@@ -965,7 +965,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.470884+09:00</t>
+          <t>2025-08-13T01:55:53.950572+09:00</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.511814+09:00</t>
+          <t>2025-08-13T01:55:53.995393+09:00</t>
         </is>
       </c>
     </row>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.565735+09:00</t>
+          <t>2025-08-13T01:55:54.047876+09:00</t>
         </is>
       </c>
     </row>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.601305+09:00</t>
+          <t>2025-08-13T01:55:54.102602+09:00</t>
         </is>
       </c>
     </row>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.656127+09:00</t>
+          <t>2025-08-13T01:55:54.145470+09:00</t>
         </is>
       </c>
     </row>
@@ -1105,7 +1105,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.708914+09:00</t>
+          <t>2025-08-13T01:55:54.190297+09:00</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.757012+09:00</t>
+          <t>2025-08-13T01:55:54.234260+09:00</t>
         </is>
       </c>
     </row>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.798914+09:00</t>
+          <t>2025-08-13T01:55:54.274789+09:00</t>
         </is>
       </c>
     </row>
@@ -1189,7 +1189,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.849248+09:00</t>
+          <t>2025-08-13T01:55:54.314644+09:00</t>
         </is>
       </c>
     </row>
@@ -1217,7 +1217,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.875817+09:00</t>
+          <t>2025-08-13T01:55:54.366434+09:00</t>
         </is>
       </c>
     </row>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.898711+09:00</t>
+          <t>2025-08-13T01:55:54.422667+09:00</t>
         </is>
       </c>
     </row>
@@ -1273,7 +1273,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.921055+09:00</t>
+          <t>2025-08-13T01:55:54.477459+09:00</t>
         </is>
       </c>
     </row>
@@ -1301,7 +1301,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.942913+09:00</t>
+          <t>2025-08-13T01:55:54.524627+09:00</t>
         </is>
       </c>
     </row>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:11.984601+09:00</t>
+          <t>2025-08-13T01:55:54.574708+09:00</t>
         </is>
       </c>
     </row>
@@ -1357,7 +1357,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:12.029066+09:00</t>
+          <t>2025-08-13T01:55:54.630188+09:00</t>
         </is>
       </c>
     </row>
@@ -1385,7 +1385,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:12.082378+09:00</t>
+          <t>2025-08-13T01:55:54.676484+09:00</t>
         </is>
       </c>
     </row>
@@ -1413,7 +1413,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:12.129823+09:00</t>
+          <t>2025-08-13T01:55:54.701121+09:00</t>
         </is>
       </c>
     </row>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:12.174372+09:00</t>
+          <t>2025-08-13T01:55:54.722034+09:00</t>
         </is>
       </c>
     </row>
@@ -1469,7 +1469,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:12.223587+09:00</t>
+          <t>2025-08-13T01:55:54.751314+09:00</t>
         </is>
       </c>
     </row>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:12.255285+09:00</t>
+          <t>2025-08-13T01:55:54.786823+09:00</t>
         </is>
       </c>
     </row>
@@ -1525,7 +1525,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:12.270980+09:00</t>
+          <t>2025-08-13T01:55:54.837621+09:00</t>
         </is>
       </c>
     </row>
@@ -1553,7 +1553,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:12.286439+09:00</t>
+          <t>2025-08-13T01:55:54.888795+09:00</t>
         </is>
       </c>
     </row>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:12.311039+09:00</t>
+          <t>2025-08-13T01:55:54.928092+09:00</t>
         </is>
       </c>
     </row>
@@ -1609,7 +1609,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:12.364914+09:00</t>
+          <t>2025-08-13T01:55:54.974682+09:00</t>
         </is>
       </c>
     </row>
@@ -1637,7 +1637,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:12.408226+09:00</t>
+          <t>2025-08-13T01:55:55.019904+09:00</t>
         </is>
       </c>
     </row>
@@ -1665,7 +1665,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:12.453413+09:00</t>
+          <t>2025-08-13T01:55:55.053073+09:00</t>
         </is>
       </c>
     </row>
@@ -1693,7 +1693,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:12.498934+09:00</t>
+          <t>2025-08-13T01:55:55.091615+09:00</t>
         </is>
       </c>
     </row>
@@ -1721,7 +1721,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:12.549301+09:00</t>
+          <t>2025-08-13T01:55:55.133436+09:00</t>
         </is>
       </c>
     </row>
@@ -1749,7 +1749,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:12.594412+09:00</t>
+          <t>2025-08-13T01:55:55.176064+09:00</t>
         </is>
       </c>
     </row>
@@ -1777,7 +1777,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:12.640991+09:00</t>
+          <t>2025-08-13T01:55:55.218868+09:00</t>
         </is>
       </c>
     </row>
@@ -1805,7 +1805,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:12.698834+09:00</t>
+          <t>2025-08-13T01:55:55.255322+09:00</t>
         </is>
       </c>
     </row>
@@ -1833,7 +1833,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:12.750484+09:00</t>
+          <t>2025-08-13T01:55:55.296021+09:00</t>
         </is>
       </c>
     </row>
@@ -1861,7 +1861,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:12.792408+09:00</t>
+          <t>2025-08-13T01:55:55.330133+09:00</t>
         </is>
       </c>
     </row>
@@ -1889,7 +1889,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:12.835984+09:00</t>
+          <t>2025-08-13T01:55:55.375853+09:00</t>
         </is>
       </c>
     </row>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:12.881891+09:00</t>
+          <t>2025-08-13T01:55:55.415729+09:00</t>
         </is>
       </c>
     </row>
@@ -1945,7 +1945,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:12.927301+09:00</t>
+          <t>2025-08-13T01:55:55.458289+09:00</t>
         </is>
       </c>
     </row>
@@ -1973,7 +1973,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:12.974489+09:00</t>
+          <t>2025-08-13T01:55:55.500614+09:00</t>
         </is>
       </c>
     </row>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:13.025787+09:00</t>
+          <t>2025-08-13T01:55:55.544531+09:00</t>
         </is>
       </c>
     </row>
@@ -2029,7 +2029,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:13.079038+09:00</t>
+          <t>2025-08-13T01:55:55.586892+09:00</t>
         </is>
       </c>
     </row>
@@ -2057,7 +2057,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:13.126204+09:00</t>
+          <t>2025-08-13T01:55:55.640140+09:00</t>
         </is>
       </c>
     </row>
@@ -2085,7 +2085,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:13.175726+09:00</t>
+          <t>2025-08-13T01:55:55.692077+09:00</t>
         </is>
       </c>
     </row>
@@ -2113,7 +2113,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:13.213477+09:00</t>
+          <t>2025-08-13T01:55:55.729388+09:00</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:13.261230+09:00</t>
+          <t>2025-08-13T01:55:55.773001+09:00</t>
         </is>
       </c>
     </row>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:13.310487+09:00</t>
+          <t>2025-08-13T01:55:55.819310+09:00</t>
         </is>
       </c>
     </row>
@@ -2197,7 +2197,7 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:13.333800+09:00</t>
+          <t>2025-08-13T01:55:55.862717+09:00</t>
         </is>
       </c>
     </row>
@@ -2225,7 +2225,7 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:13.377986+09:00</t>
+          <t>2025-08-13T01:55:55.910090+09:00</t>
         </is>
       </c>
     </row>
@@ -2253,7 +2253,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:13.415860+09:00</t>
+          <t>2025-08-13T01:55:55.952182+09:00</t>
         </is>
       </c>
     </row>
@@ -2281,7 +2281,7 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:13.469743+09:00</t>
+          <t>2025-08-13T01:55:55.994977+09:00</t>
         </is>
       </c>
     </row>
@@ -2309,7 +2309,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:13.521355+09:00</t>
+          <t>2025-08-13T01:55:56.040061+09:00</t>
         </is>
       </c>
     </row>
@@ -2337,7 +2337,7 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:13.573687+09:00</t>
+          <t>2025-08-13T01:55:56.090615+09:00</t>
         </is>
       </c>
     </row>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:13.616695+09:00</t>
+          <t>2025-08-13T01:55:56.138924+09:00</t>
         </is>
       </c>
     </row>
@@ -2393,7 +2393,7 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:13.668394+09:00</t>
+          <t>2025-08-13T01:55:56.188462+09:00</t>
         </is>
       </c>
     </row>
@@ -2421,7 +2421,7 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:13.703724+09:00</t>
+          <t>2025-08-13T01:55:56.238163+09:00</t>
         </is>
       </c>
     </row>
@@ -2449,7 +2449,7 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:13.750056+09:00</t>
+          <t>2025-08-13T01:55:56.278651+09:00</t>
         </is>
       </c>
     </row>
@@ -2477,7 +2477,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:13.791104+09:00</t>
+          <t>2025-08-13T01:55:56.309434+09:00</t>
         </is>
       </c>
     </row>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:13.841915+09:00</t>
+          <t>2025-08-13T01:55:56.336357+09:00</t>
         </is>
       </c>
     </row>
@@ -2533,7 +2533,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:13.879724+09:00</t>
+          <t>2025-08-13T01:55:56.377485+09:00</t>
         </is>
       </c>
     </row>
@@ -2561,7 +2561,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:13.925609+09:00</t>
+          <t>2025-08-13T01:55:56.429566+09:00</t>
         </is>
       </c>
     </row>
@@ -2589,7 +2589,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:13.980401+09:00</t>
+          <t>2025-08-13T01:55:56.478229+09:00</t>
         </is>
       </c>
     </row>
@@ -2617,7 +2617,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:14.022233+09:00</t>
+          <t>2025-08-13T01:55:56.514014+09:00</t>
         </is>
       </c>
     </row>
@@ -2645,7 +2645,7 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:14.073894+09:00</t>
+          <t>2025-08-13T01:55:56.566186+09:00</t>
         </is>
       </c>
     </row>
@@ -2673,7 +2673,7 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:14.123583+09:00</t>
+          <t>2025-08-13T01:55:56.618902+09:00</t>
         </is>
       </c>
     </row>
@@ -2701,7 +2701,7 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:14.176386+09:00</t>
+          <t>2025-08-13T01:55:56.667213+09:00</t>
         </is>
       </c>
     </row>
@@ -2729,7 +2729,7 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:14.214595+09:00</t>
+          <t>2025-08-13T01:55:56.711279+09:00</t>
         </is>
       </c>
     </row>
@@ -2757,7 +2757,7 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:14.243276+09:00</t>
+          <t>2025-08-13T01:55:56.751206+09:00</t>
         </is>
       </c>
     </row>
@@ -2785,7 +2785,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:14.278160+09:00</t>
+          <t>2025-08-13T01:55:56.795307+09:00</t>
         </is>
       </c>
     </row>
@@ -2813,7 +2813,7 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:14.325737+09:00</t>
+          <t>2025-08-13T01:55:56.835927+09:00</t>
         </is>
       </c>
     </row>
@@ -2841,7 +2841,7 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:14.369012+09:00</t>
+          <t>2025-08-13T01:55:56.875197+09:00</t>
         </is>
       </c>
     </row>
@@ -2869,7 +2869,7 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:14.415305+09:00</t>
+          <t>2025-08-13T01:55:56.922872+09:00</t>
         </is>
       </c>
     </row>
@@ -2897,7 +2897,7 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:14.468018+09:00</t>
+          <t>2025-08-13T01:55:56.966119+09:00</t>
         </is>
       </c>
     </row>
@@ -2925,7 +2925,7 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:14.520226+09:00</t>
+          <t>2025-08-13T01:55:57.017825+09:00</t>
         </is>
       </c>
     </row>
@@ -2953,7 +2953,7 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:14.570467+09:00</t>
+          <t>2025-08-13T01:55:57.060157+09:00</t>
         </is>
       </c>
     </row>
@@ -2981,7 +2981,7 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:14.623753+09:00</t>
+          <t>2025-08-13T01:55:57.092958+09:00</t>
         </is>
       </c>
     </row>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:14.673408+09:00</t>
+          <t>2025-08-13T01:55:57.122578+09:00</t>
         </is>
       </c>
     </row>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:14.722752+09:00</t>
+          <t>2025-08-13T01:55:57.145922+09:00</t>
         </is>
       </c>
     </row>
@@ -3065,7 +3065,7 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:14.760042+09:00</t>
+          <t>2025-08-13T01:55:57.192625+09:00</t>
         </is>
       </c>
     </row>
@@ -3093,7 +3093,7 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:14.777575+09:00</t>
+          <t>2025-08-13T01:55:57.240699+09:00</t>
         </is>
       </c>
     </row>
@@ -3121,7 +3121,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:14.804877+09:00</t>
+          <t>2025-08-13T01:55:57.293206+09:00</t>
         </is>
       </c>
     </row>
@@ -3149,7 +3149,7 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:14.857909+09:00</t>
+          <t>2025-08-13T01:55:57.337886+09:00</t>
         </is>
       </c>
     </row>
@@ -3177,7 +3177,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:14.907026+09:00</t>
+          <t>2025-08-13T01:55:57.385130+09:00</t>
         </is>
       </c>
     </row>
@@ -3205,7 +3205,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:14.958095+09:00</t>
+          <t>2025-08-13T01:55:57.436720+09:00</t>
         </is>
       </c>
     </row>
@@ -3233,7 +3233,7 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:14.998695+09:00</t>
+          <t>2025-08-13T01:55:57.493456+09:00</t>
         </is>
       </c>
     </row>
@@ -3261,7 +3261,7 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>2025-08-13T01:44:15.044392+09:00</t>
+          <t>2025-08-13T01:55:57.531219+09:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Oliveyoung rankings with latest product order and timestamps
Co-authored-by: jongpard <jongpard@gmail.com>
</commit_message>
<xml_diff>
--- a/oliveyoung_rankings_2025-08-13.xlsx
+++ b/oliveyoung_rankings_2025-08-13.xlsx
@@ -489,7 +489,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:53.253319+09:00</t>
+          <t>2025-08-13T02:16:09.334730+09:00</t>
         </is>
       </c>
     </row>
@@ -499,25 +499,25 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[쓰까르3일마켓] [리뷰이벤트/크림본품증정] 메디큐브 에이지알 부스터프로 미니플러스 베이지/핑크</t>
+          <t>[재구매1위/장벽크림] 일리윤 세라마이드아토 집중크림 150ML*2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>107,500원 ~</t>
+          <t>18,900원</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>107500</v>
+        <v>18900</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231154&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=2</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000217767&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=2</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:53.285291+09:00</t>
+          <t>2025-08-13T02:16:09.381622+09:00</t>
         </is>
       </c>
     </row>
@@ -527,25 +527,25 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[재구매1위/장벽크림] 일리윤 세라마이드아토 집중크림 150ML*2</t>
+          <t>[쓰까르3일마켓] [리뷰이벤트/크림본품증정] 메디큐브 에이지알 부스터프로 미니플러스 베이지/핑크</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>18,900원</t>
+          <t>107,500원 ~</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>18900</v>
+        <v>107500</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000217767&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=3</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231154&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=3</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:53.321593+09:00</t>
+          <t>2025-08-13T02:16:09.422530+09:00</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:53.367439+09:00</t>
+          <t>2025-08-13T02:16:09.458947+09:00</t>
         </is>
       </c>
     </row>
@@ -601,7 +601,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:53.423481+09:00</t>
+          <t>2025-08-13T02:16:09.504142+09:00</t>
         </is>
       </c>
     </row>
@@ -629,7 +629,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:53.482434+09:00</t>
+          <t>2025-08-13T02:16:09.539674+09:00</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:53.538615+09:00</t>
+          <t>2025-08-13T02:16:09.592912+09:00</t>
         </is>
       </c>
     </row>
@@ -685,7 +685,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:53.585426+09:00</t>
+          <t>2025-08-13T02:16:09.642444+09:00</t>
         </is>
       </c>
     </row>
@@ -695,25 +695,25 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[천만돌파/1+1] 비플레인 녹두 약산성 클렌징폼 160ml+160ml 기획</t>
+          <t>[고민영PICK/한정기획] 아벤느 이드랑스 에센스 인 로션 200ml 한정 기획 (+100ml*2) *수분 충전</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>23,500원</t>
+          <t>27,900원</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>23500</v>
+        <v>27900</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000222605&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=9</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230424&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=9</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:53.625601+09:00</t>
+          <t>2025-08-13T02:16:09.691991+09:00</t>
         </is>
       </c>
     </row>
@@ -723,25 +723,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[고민영PICK/한정기획] 아벤느 이드랑스 에센스 인 로션 200ml 한정 기획 (+100ml*2) *수분 충전</t>
+          <t>[천만돌파/1+1] 비플레인 녹두 약산성 클렌징폼 160ml+160ml 기획</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>27,900원</t>
+          <t>23,500원</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>27900</v>
+        <v>23500</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230424&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=10</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000222605&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=10</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:53.665736+09:00</t>
+          <t>2025-08-13T02:16:09.732831+09:00</t>
         </is>
       </c>
     </row>
@@ -751,25 +751,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[푸디젠 PICK | 리뷰 이벤트] 구달 청귤 비타C 잡티케어 세럼 알파 50ml 리필 기획 (+크림 10ml)</t>
+          <t>[8월 펀딩][당0g대] 크런틴 크런치볼 단백질쉐이크 초코이즈백 3box(15팩)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>28,500원</t>
+          <t>57,900원</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>28500</v>
+        <v>57900</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230654&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=11</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=B000000227402&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=11</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:53.685832+09:00</t>
+          <t>2025-08-13T02:16:09.750559+09:00</t>
         </is>
       </c>
     </row>
@@ -779,25 +779,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[8월 펀딩][당0g대] 크런틴 크런치볼 단백질쉐이크 초코이즈백 3box(15팩)</t>
+          <t>[푸디젠 PICK | 리뷰 이벤트] 구달 청귤 비타C 잡티케어 세럼 알파 50ml 리필 기획 (+크림 10ml)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>57,900원</t>
+          <t>28,500원</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>57900</v>
+        <v>28500</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=B000000227402&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=12</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230654&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=12</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:53.704012+09:00</t>
+          <t>2025-08-13T02:16:09.765067+09:00</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:53.722664+09:00</t>
+          <t>2025-08-13T02:16:09.781720+09:00</t>
         </is>
       </c>
     </row>
@@ -835,25 +835,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[3시간팩] 바이오던스 리얼 딥 마스크 7매 (콜라겐, 세라놀, 비타, 씨켈프)</t>
+          <t>[8월 올영픽/NO.1 미스트세럼] 달바 퍼스트 스프레이 세럼 100ml 2개 기획</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>28,900원 ~</t>
+          <t>32,900원</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>28900</v>
+        <v>32900</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000221807&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=14</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000179685&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=14</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:53.767675+09:00</t>
+          <t>2025-08-13T02:16:09.804461+09:00</t>
         </is>
       </c>
     </row>
@@ -863,25 +863,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[8월 올영픽/NO.1 미스트세럼] 달바 퍼스트 스프레이 세럼 100ml 2개 기획</t>
+          <t>[7일특가/좌두pick] 마미케어 바다포도 모공앰플 50ml</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>32,900원</t>
+          <t>13,800원</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>32900</v>
+        <v>13800</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000179685&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=15</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000224295&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=15</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:53.823886+09:00</t>
+          <t>2025-08-13T02:16:09.841858+09:00</t>
         </is>
       </c>
     </row>
@@ -891,25 +891,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[7일특가/좌두pick] 마미케어 바다포도 모공앰플 50ml</t>
+          <t>[NEW] 아누아 TXA 나이아신 흔적 세럼 30ml 2입</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>13,800원</t>
+          <t>27,500원</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>13800</v>
+        <v>27500</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000224295&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=16</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000226201&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=16</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:53.859082+09:00</t>
+          <t>2025-08-13T02:16:09.891196+09:00</t>
         </is>
       </c>
     </row>
@@ -919,25 +919,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[4년연속1위/블랙헤드OUT] 마녀공장 퓨어 클렌징 오일 300ml 기획 (+25mlx2)</t>
+          <t>[3시간팩] 바이오던스 리얼 딥 마스크 7매 (콜라겐, 세라놀, 비타, 씨켈프)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>19,900원</t>
+          <t>28,900원 ~</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>19900</v>
+        <v>28900</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000199588&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=17</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000221807&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=17</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:53.909603+09:00</t>
+          <t>2025-08-13T02:16:09.936987+09:00</t>
         </is>
       </c>
     </row>
@@ -947,25 +947,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[꼬마마법사 레미 콜라보/100% 리뷰이벤트] 키스미 아이 블러 이펙트 틴트 3.5g 7종 (올영 단독 선론칭)</t>
+          <t>[4년연속1위/블랙헤드OUT] 마녀공장 퓨어 클렌징 오일 300ml 기획 (+25mlx2)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>12,900원 ~</t>
+          <t>19,900원</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>12900</v>
+        <v>19900</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000214282&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=18</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000199588&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=18</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:53.950572+09:00</t>
+          <t>2025-08-13T02:16:09.982056+09:00</t>
         </is>
       </c>
     </row>
@@ -975,25 +975,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>[NEW] 아누아 TXA 나이아신 흔적 세럼 30ml 2입</t>
+          <t>[꼬마마법사 레미 콜라보/100% 리뷰이벤트] 키스미 아이 블러 이펙트 틴트 3.5g 7종 (올영 단독 선론칭)</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>27,500원</t>
+          <t>12,900원 ~</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>27500</v>
+        <v>12900</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000226201&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=19</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000214282&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=19</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:53.995393+09:00</t>
+          <t>2025-08-13T02:16:10.032620+09:00</t>
         </is>
       </c>
     </row>
@@ -1003,25 +1003,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[3년 연속 1위] 어노브 딥 데미지 헤어 트리트먼트 EX 320ml 더블/듀오 기획 3종 택1</t>
+          <t>[시드니픽/8월] 아벤느 클리낭스 클렌징젤 400ml 더블기획 (클리낭스 세럼 2ml + 클리낭스아쿠아크림인젤 2ml)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>29,800원 ~</t>
+          <t>28,900원</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>29800</v>
+        <v>28900</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000171423&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=20</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230423&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=20</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:54.047876+09:00</t>
+          <t>2025-08-13T02:16:10.079682+09:00</t>
         </is>
       </c>
     </row>
@@ -1031,25 +1031,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>[피지클렌징] 마몽드 어메이징 딥 민트 클렌징밤 90ml 기획 (+폼 30ml)</t>
+          <t>[8월올영픽] 아비브 어성초 흔적 에센스 패드 클리어터치 140매 (70매+70매 리필)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>16,000원</t>
+          <t>26,600원</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>16000</v>
+        <v>26600</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000198831&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=21</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000219555&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=21</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:54.102602+09:00</t>
+          <t>2025-08-13T02:16:10.125703+09:00</t>
         </is>
       </c>
     </row>
@@ -1059,25 +1059,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>[8월올영픽] 아비브 어성초 흔적 에센스 패드 클리어터치 140매 (70매+70매 리필)</t>
+          <t>[3년 연속 1위] 어노브 딥 데미지 헤어 트리트먼트 EX 320ml 더블/듀오 기획 3종 택1</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>26,600원</t>
+          <t>29,800원 ~</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>26600</v>
+        <v>29800</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000219555&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=22</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000171423&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=22</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:54.145470+09:00</t>
+          <t>2025-08-13T02:16:10.169112+09:00</t>
         </is>
       </c>
     </row>
@@ -1087,25 +1087,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>[시드니픽/8월] 아벤느 클리낭스 클렌징젤 400ml 더블기획 (클리낭스 세럼 2ml + 클리낭스아쿠아크림인젤 2ml)</t>
+          <t>[피지클렌징] 마몽드 어메이징 딥 민트 클렌징밤 90ml 기획 (+폼 30ml)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>28,900원</t>
+          <t>16,000원</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>28900</v>
+        <v>16000</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230423&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=23</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000198831&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=23</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:54.190297+09:00</t>
+          <t>2025-08-13T02:16:10.222219+09:00</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:54.234260+09:00</t>
+          <t>2025-08-13T02:16:10.272661+09:00</t>
         </is>
       </c>
     </row>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:54.274789+09:00</t>
+          <t>2025-08-13T02:16:10.319028+09:00</t>
         </is>
       </c>
     </row>
@@ -1171,25 +1171,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>[1+1 더블기획] 라곰 셀럽 마이크로 수분 폼 클렌저 120ml x 2</t>
+          <t>라로슈포제 시카플라스트 밤 B5+ 100ml 기획 (+히알루 B5 세럼 1.5ml*2 증정)</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>24,650원</t>
+          <t>36,000원</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>24650</v>
+        <v>36000</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230821&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=26</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000226997&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=26</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:54.314644+09:00</t>
+          <t>2025-08-13T02:16:10.354521+09:00</t>
         </is>
       </c>
     </row>
@@ -1199,25 +1199,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>라로슈포제 시카플라스트 밤 B5+ 100ml 기획 (+히알루 B5 세럼 1.5ml*2 증정)</t>
+          <t>세노비스 밀크씨슬 120캡슐 (4개월분)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>36,000원</t>
+          <t>25,000원</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>36000</v>
+        <v>25000</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000226997&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=27</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000129053&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=27</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:54.366434+09:00</t>
+          <t>2025-08-13T02:16:10.409064+09:00</t>
         </is>
       </c>
     </row>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:54.422667+09:00</t>
+          <t>2025-08-13T02:16:10.466378+09:00</t>
         </is>
       </c>
     </row>
@@ -1255,25 +1255,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>[14년연속 1위] 메디힐 에센셜 마스크팩 1매 고기능 7종 택1</t>
+          <t>[8월 올영픽/하트거울증정] 이니스프리 레티놀 시카 흔적 앰플 30ml 더블 기획</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1,000원 ~</t>
+          <t>28,710원</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>1000</v>
+        <v>28710</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000217620&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=29</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230208&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=29</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:54.477459+09:00</t>
+          <t>2025-08-13T02:16:10.518220+09:00</t>
         </is>
       </c>
     </row>
@@ -1283,25 +1283,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>[8월 올영픽/하트거울증정] 이니스프리 레티놀 시카 흔적 앰플 30ml 더블 기획</t>
+          <t>[14년연속 1위] 메디힐 에센셜 마스크팩 1매 고기능 7종 택1</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>28,710원</t>
+          <t>1,000원 ~</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>28710</v>
+        <v>1000</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230208&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=30</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000217620&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=30</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:54.524627+09:00</t>
+          <t>2025-08-13T02:16:10.555343+09:00</t>
         </is>
       </c>
     </row>
@@ -1311,25 +1311,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>세노비스 밀크씨슬 120캡슐 (4개월분)</t>
+          <t>[1+1 더블기획] 라곰 셀럽 마이크로 수분 폼 클렌저 120ml x 2</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>25,000원</t>
+          <t>24,650원</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>25000</v>
+        <v>24650</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000129053&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=31</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230821&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=31</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:54.574708+09:00</t>
+          <t>2025-08-13T02:16:10.604213+09:00</t>
         </is>
       </c>
     </row>
@@ -1339,25 +1339,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>[8월올영픽/Oiad x 어프어프 콜라보] 오아드 립티크 9종 단품/기획</t>
+          <t>[KBO 파우치 증정] 메디힐 네모패드 더블기획 3종 골라담기(마데카소사이드, PDRN, 티트리)(KBO 에디션)</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>21,900원 ~</t>
+          <t>28,900원 ~</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>21900</v>
+        <v>28900</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000218834&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=32</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231048&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=32</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:54.630188+09:00</t>
+          <t>2025-08-13T02:16:10.659729+09:00</t>
         </is>
       </c>
     </row>
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>바이오더마 센시비오 H2O 850ml(클렌징워터)</t>
+          <t>[8월올영픽/Oiad x 어프어프 콜라보] 오아드 립티크 9종 단품/기획</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>24,610원</t>
+          <t>21,900원 ~</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>24610</v>
+        <v>21900</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000130319&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=33</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000218834&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=33</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:54.676484+09:00</t>
+          <t>2025-08-13T02:16:10.711872+09:00</t>
         </is>
       </c>
     </row>
@@ -1395,25 +1395,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>[단독특가] 푸드올로지 지중해 레몬버베나 500mg 60정 (1개월분)</t>
+          <t>[덱스 PICK] 오브제 내추럴 커버 로션 50g 단품/기획(+미니어처 10ml)</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>38,100원</t>
+          <t>26,510원 ~</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>38100</v>
+        <v>26510</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230972&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=34</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000204975&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=34</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:54.701121+09:00</t>
+          <t>2025-08-13T02:16:10.750968+09:00</t>
         </is>
       </c>
     </row>
@@ -1423,25 +1423,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>[KBO 파우치 증정] 메디힐 네모패드 더블기획 3종 골라담기(마데카소사이드, PDRN, 티트리)(KBO 에디션)</t>
+          <t>[단독특가] 푸드올로지 지중해 레몬버베나 500mg 60정 (1개월분)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>28,900원 ~</t>
+          <t>38,100원</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>28900</v>
+        <v>38100</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231048&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=35</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230972&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=35</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:54.722034+09:00</t>
+          <t>2025-08-13T02:16:10.769486+09:00</t>
         </is>
       </c>
     </row>
@@ -1451,25 +1451,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>[8월 올영픽/핑구콜라보] 코스노리 화이트닝 드레스 비건 톤업크림 (단품/기획)</t>
+          <t>[8월 올영픽/가나디콜라보] 토리든 다이브인 저분자 히알루론산 수딩 크림 100ml 가나디 더블 기획 (+파우치 키링)</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>16,000원 ~</t>
+          <t>30,000원</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>16000</v>
+        <v>30000</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000017135&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=36</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230832&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=36</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:54.751314+09:00</t>
+          <t>2025-08-13T02:16:10.786956+09:00</t>
         </is>
       </c>
     </row>
@@ -1479,25 +1479,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>[율리 PICK/5+1매 한정기획] 아이오페 레티놀 세럼 인 겔 마스크 기획</t>
+          <t>[1+1/단독기획] 메디힐 마데카소사이드 흔적 리페어 세럼 40+40ml 더블 기획</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>23,600원</t>
+          <t>22,900원</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>23600</v>
+        <v>22900</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000224510&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=37</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000211119&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=37</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:54.786823+09:00</t>
+          <t>2025-08-13T02:16:10.820134+09:00</t>
         </is>
       </c>
     </row>
@@ -1507,25 +1507,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>[파격특가] 질레트 랩스 딥클렌징바 면도기 (핸들+1입날)</t>
+          <t>[율리 PICK/5+1매 한정기획] 아이오페 레티놀 세럼 인 겔 마스크 기획</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>9,900원</t>
+          <t>23,600원</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>9900</v>
+        <v>23600</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000174122&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=38</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000224510&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=38</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:54.837621+09:00</t>
+          <t>2025-08-13T02:16:10.867848+09:00</t>
         </is>
       </c>
     </row>
@@ -1535,25 +1535,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>[8월 올영픽/가나디콜라보] 토리든 다이브인 저분자 히알루론산 수딩 크림 100ml 가나디 더블 기획 (+파우치 키링)</t>
+          <t>[8월 올영픽/핑구콜라보] 코스노리 화이트닝 드레스 비건 톤업크림 (단품/기획)</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>30,000원</t>
+          <t>16,000원 ~</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>30000</v>
+        <v>16000</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230832&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=39</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000017135&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=39</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:54.888795+09:00</t>
+          <t>2025-08-13T02:16:10.908556+09:00</t>
         </is>
       </c>
     </row>
@@ -1563,25 +1563,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>[덱스 PICK] 오브제 내추럴 커버 로션 50g 단품/기획(+미니어처 10ml)</t>
+          <t>수이사이 뷰티 클리어 파우더워시 산리오 콜라보 6종 택1</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>26,510원 ~</t>
+          <t>19,440원 ~</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>26510</v>
+        <v>19440</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000204975&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=40</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230670&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=40</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:54.928092+09:00</t>
+          <t>2025-08-13T02:16:10.939302+09:00</t>
         </is>
       </c>
     </row>
@@ -1591,25 +1591,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>[25ml 추가증정] 휩드 비건 팩클렌저 130g 기획 3종 (머그트리/무화버터/유자몽)</t>
+          <t>[NEW/리뉴얼] 컬러그램 누디 블러 틴트 18 COLOR</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>19,700원 ~</t>
+          <t>8,300원 ~</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>19700</v>
+        <v>8300</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000217511&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=41</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230581&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=41</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:54.974682+09:00</t>
+          <t>2025-08-13T02:16:10.977652+09:00</t>
         </is>
       </c>
     </row>
@@ -1619,25 +1619,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>[3년연속1등] 라보에이치 두피강화샴푸 750+125ML(단품/기획)</t>
+          <t>[25ml 추가증정] 휩드 비건 팩클렌저 130g 기획 3종 (머그트리/무화버터/유자몽)</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>25,900원 ~</t>
+          <t>19,700원 ~</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>25900</v>
+        <v>19700</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000149501&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=42</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000217511&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=42</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.019904+09:00</t>
+          <t>2025-08-13T02:16:11.030158+09:00</t>
         </is>
       </c>
     </row>
@@ -1647,25 +1647,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>[1+1/단독기획] 메디힐 마데카소사이드 흔적 리페어 세럼 40+40ml 더블 기획</t>
+          <t>[1+1한정기획/열감진정] 스킨푸드 캐롯 카로틴 카밍 워터 패드 60매 더블기획 (본품+본품)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>22,900원</t>
+          <t>26,900원</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>22900</v>
+        <v>26900</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000211119&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=43</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000224932&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=43</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.053073+09:00</t>
+          <t>2025-08-13T02:16:11.067455+09:00</t>
         </is>
       </c>
     </row>
@@ -1675,25 +1675,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>[1+1한정기획/열감진정] 스킨푸드 캐롯 카로틴 카밍 워터 패드 60매 더블기획 (본품+본품)</t>
+          <t>[뷰티디바이스 1위] [광채토닝 메디큐브 부스터프로 쿠로미 에디션(+쿠로미헤드캡+세안밴드+디바이스클리너+스티커2종)</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>26,900원</t>
+          <t>349,000원</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>26900</v>
+        <v>349000</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000224932&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=44</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000224654&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=44</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.091615+09:00</t>
+          <t>2025-08-13T02:16:11.105379+09:00</t>
         </is>
       </c>
     </row>
@@ -1703,25 +1703,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>[산리오캐릭터즈] 롬앤 더 쥬시 래스팅 틴트 (+쉐이킹키링증정) 단품/기획</t>
+          <t>바이오더마 시카비오 포마드 100ml(리페어 리치 밤)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>13,000원 ~</t>
+          <t>28,500원</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>13000</v>
+        <v>28500</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000213153&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=45</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000134691&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=45</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.133436+09:00</t>
+          <t>2025-08-13T02:16:11.132373+09:00</t>
         </is>
       </c>
     </row>
@@ -1731,25 +1731,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>[NEW/리뉴얼] 컬러그램 누디 블러 틴트 18 COLOR</t>
+          <t>[파격특가] 질레트 랩스 딥클렌징바 면도기 (핸들+1입날)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>8,300원 ~</t>
+          <t>9,900원</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>8300</v>
+        <v>9900</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230581&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=46</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000174122&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=46</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.176064+09:00</t>
+          <t>2025-08-13T02:16:11.157314+09:00</t>
         </is>
       </c>
     </row>
@@ -1759,25 +1759,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>바이오더마 시카비오 포마드 100ml(리페어 리치 밤)</t>
+          <t>[파격특가] 피지오겔 시카밸런스 포맨 카밍 크림 70ml</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>28,500원</t>
+          <t>9,900원</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>28500</v>
+        <v>9900</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000134691&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=47</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000211188&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=47</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.218868+09:00</t>
+          <t>2025-08-13T02:16:11.175181+09:00</t>
         </is>
       </c>
     </row>
@@ -1787,25 +1787,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>[8월 올영픽]오브제 포어 제로 오일 컨트롤 선스틱 18g</t>
+          <t>바이오더마 센시비오 H2O 850ml(클렌징워터)</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>17,800원</t>
+          <t>24,610원</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>17800</v>
+        <v>24610</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000225044&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=48</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000130319&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=48</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.255322+09:00</t>
+          <t>2025-08-13T02:16:11.193860+09:00</t>
         </is>
       </c>
     </row>
@@ -1815,25 +1815,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>[8월올영픽/겔마스크] 메디힐 하이퍼 마스크 5+1매 2종 택 1 [콜라겐/히알루론산]</t>
+          <t>[산리오캐릭터즈] 롬앤 더 쥬시 래스팅 틴트 (+쉐이킹키링증정) 단품/기획</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>16,200원 ~</t>
+          <t>13,000원 ~</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>16200</v>
+        <v>13000</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000216349&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=49</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000213153&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=49</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.296021+09:00</t>
+          <t>2025-08-13T02:16:11.224068+09:00</t>
         </is>
       </c>
     </row>
@@ -1843,25 +1843,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>[파격특가] 피지오겔 시카밸런스 포맨 카밍 크림 70ml</t>
+          <t>[3년연속1등] 라보에이치 두피강화샴푸 750+125ML(단품/기획)</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>9,900원</t>
+          <t>25,900원 ~</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>9900</v>
+        <v>25900</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000211188&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=50</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000149501&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=50</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.330133+09:00</t>
+          <t>2025-08-13T02:16:11.268140+09:00</t>
         </is>
       </c>
     </row>
@@ -1871,25 +1871,25 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>[뷰티디바이스 1위] [광채토닝 메디큐브 부스터프로 쿠로미 에디션(+쿠로미헤드캡+세안밴드+디바이스클리너+스티커2종)</t>
+          <t>[유시은pick/1등홈경락템] 마미케어 EMS브이쎄라 (화이트/핑크/NEW 퍼플에디션) (+전용 부스팅젤 본품 증정)</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>349,000원</t>
+          <t>99,000원 ~</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>349000</v>
+        <v>99000</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000224654&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=51</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=B000000224350&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=51</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.375853+09:00</t>
+          <t>2025-08-13T02:16:11.314313+09:00</t>
         </is>
       </c>
     </row>
@@ -1899,25 +1899,25 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>[태닝포차코/한정] 바이탈뷰티 메타그린 슬림업 60정 기획 (+포차코 파우치 증정)</t>
+          <t>[8월 올영픽]오브제 포어 제로 오일 컨트롤 선스틱 18g</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>28,320원</t>
+          <t>17,800원</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>28320</v>
+        <v>17800</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000229143&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=52</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000225044&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=52</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.415729+09:00</t>
+          <t>2025-08-13T02:16:11.356490+09:00</t>
         </is>
       </c>
     </row>
@@ -1927,25 +1927,25 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>[올영픽/피지아웃/화잘먹 수분천재세럼] 에스네이처 아쿠아 스쿠알란 세럼 50ml 기획(+50ml 리필+수분크림10ml)</t>
+          <t>[1등 속눈썹/NEW] 코링코 톡톡하라 노글루 속눈썹 11종 택1</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>21,700원</t>
+          <t>13,900원 ~</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>21700</v>
+        <v>13900</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000188004&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=53</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000213569&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=53</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.458289+09:00</t>
+          <t>2025-08-13T02:16:11.387148+09:00</t>
         </is>
       </c>
     </row>
@@ -1955,25 +1955,25 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>[한겹밀착커버] 에이프릴스킨 히어로쿠션 핑크에디션(본품+리필+퍼프2개)</t>
+          <t>포뷰트 두피 타투15g 블랙 (+추영우 포토카드 증정 이벤트)</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>24,900원 ~</t>
+          <t>16,800원</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>24900</v>
+        <v>16800</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000163765&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=54</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000223552&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=54</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.500614+09:00</t>
+          <t>2025-08-13T02:16:11.433238+09:00</t>
         </is>
       </c>
     </row>
@@ -1983,25 +1983,25 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>(50%용량증정)에스트라 더마UV365 장벽수분 무기자차 선크림 40ml+20ml 기획</t>
+          <t>[올영픽/피지아웃/화잘먹 수분천재세럼] 에스네이처 아쿠아 스쿠알란 세럼 50ml 기획(+50ml 리필+수분크림10ml)</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>24,800원</t>
+          <t>21,700원</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>24800</v>
+        <v>21700</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000206826&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=55</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000188004&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=55</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.544531+09:00</t>
+          <t>2025-08-13T02:16:11.476543+09:00</t>
         </is>
       </c>
     </row>
@@ -2011,25 +2011,25 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>[8월올영픽/포켓몬 에디션]성분에디터 그린토마토 NMN 포어 리프팅 앰플 40ml 더블 기획 (+키링 파우치)</t>
+          <t>[8월 올영픽] [유시몰X헌터] 장화스탠더+퍼플코렉터 미백치약 106g*2</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>22,800원</t>
+          <t>25,900원</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>22800</v>
+        <v>25900</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230914&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=56</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230647&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=56</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.586892+09:00</t>
+          <t>2025-08-13T02:16:11.511086+09:00</t>
         </is>
       </c>
     </row>
@@ -2039,25 +2039,25 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>포뷰트 두피 타투15g 블랙 (+추영우 포토카드 증정 이벤트)</t>
+          <t>[NEW/8월올영픽] 플르부아 디퓨저 200ml &amp; 센티드 타블렛(퍼퓸 샤쉐) 단품/기획</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>16,800원</t>
+          <t>26,300원 ~</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>16800</v>
+        <v>26300</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000223552&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=57</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000202553&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=57</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.640140+09:00</t>
+          <t>2025-08-13T02:16:11.545366+09:00</t>
         </is>
       </c>
     </row>
@@ -2067,25 +2067,25 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>[NEW/8월올영픽] 플르부아 디퓨저 200ml &amp; 센티드 타블렛(퍼퓸 샤쉐) 단품/기획</t>
+          <t>[8월올영픽/포켓몬 에디션]성분에디터 그린토마토 NMN 포어 리프팅 앰플 40ml 더블 기획 (+키링 파우치)</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>26,300원 ~</t>
+          <t>22,800원</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>26300</v>
+        <v>22800</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000202553&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=58</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230914&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=58</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.692077+09:00</t>
+          <t>2025-08-13T02:16:11.565847+09:00</t>
         </is>
       </c>
     </row>
@@ -2095,25 +2095,25 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>[8월 올영픽] [유시몰X헌터] 장화스탠더+퍼플코렉터 미백치약 106g*2</t>
+          <t>[1등진정/크라이베이비 이벤트] 파넬 시카마누 92세럼 더블기획(30ml+30ml)</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>25,900원</t>
+          <t>22,900원</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>25900</v>
+        <v>22900</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230647&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=59</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000189713&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=59</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.729388+09:00</t>
+          <t>2025-08-13T02:16:11.582181+09:00</t>
         </is>
       </c>
     </row>
@@ -2123,25 +2123,25 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>[수분진정/세럼증정] 닥터지 레드 블레미쉬 클리어 수딩 크림 70ml 증정기획 2종</t>
+          <t>[태닝포차코/한정] 바이탈뷰티 메타그린 슬림업 60정 기획 (+포차코 파우치 증정)</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>27,600원 ~</t>
+          <t>28,320원</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>27600</v>
+        <v>28320</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000164615&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=60</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000229143&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=60</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.773001+09:00</t>
+          <t>2025-08-13T02:16:11.604781+09:00</t>
         </is>
       </c>
     </row>
@@ -2151,25 +2151,25 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>[유시은pick/1등홈경락템] 마미케어 EMS브이쎄라 (화이트/핑크/NEW 퍼플에디션) (+전용 부스팅젤 본품 증정)</t>
+          <t>[8월올영픽/겔마스크] 메디힐 하이퍼 마스크 5+1매 2종 택 1 [콜라겐/히알루론산]</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>99,000원 ~</t>
+          <t>16,200원 ~</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>99000</v>
+        <v>16200</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=B000000224350&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=61</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000216349&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=61</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.819310+09:00</t>
+          <t>2025-08-13T02:16:11.645656+09:00</t>
         </is>
       </c>
     </row>
@@ -2179,25 +2179,25 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>[1등진정/크라이베이비 이벤트] 파넬 시카마누 92세럼 더블기획(30ml+30ml)</t>
+          <t>[한겹밀착커버] 에이프릴스킨 히어로쿠션 핑크에디션(본품+리필+퍼프2개)</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>22,900원</t>
+          <t>24,900원 ~</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>22900</v>
+        <v>24900</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000189713&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=62</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000163765&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=62</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.862717+09:00</t>
+          <t>2025-08-13T02:16:11.681822+09:00</t>
         </is>
       </c>
     </row>
@@ -2207,25 +2207,25 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>수이사이 뷰티 클리어 파우더워시 산리오 콜라보 6종 택1</t>
+          <t>플라이밀 단백질쉐이크 45g 9종 택1</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>19,440원 ~</t>
+          <t>2,970원 ~</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>19440</v>
+        <v>2970</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230670&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=63</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000190168&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=63</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.910090+09:00</t>
+          <t>2025-08-13T02:16:11.709487+09:00</t>
         </is>
       </c>
     </row>
@@ -2235,25 +2235,25 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>[1등 속눈썹/NEW] 코링코 톡톡하라 노글루 속눈썹 11종 택1</t>
+          <t>[수분진정] 아비브 어성초 카밍 토너 스킨부스터 더블 기획 (200ml+200ml)</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>13,900원 ~</t>
+          <t>27,300원</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>13900</v>
+        <v>27300</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000213569&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=64</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000155253&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=64</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.952182+09:00</t>
+          <t>2025-08-13T02:16:11.750866+09:00</t>
         </is>
       </c>
     </row>
@@ -2263,25 +2263,25 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>[1등미백앰플/대용량기획]메디큐브 PDRN 핑크 펩타이드 앰플 30ml 리필기획(본품 30ML+리필 50ML)</t>
+          <t>(50%용량증정)에스트라 더마UV365 장벽수분 무기자차 선크림 40ml+20ml 기획</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>25,900원</t>
+          <t>24,800원</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>25900</v>
+        <v>24800</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000226498&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=65</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000206826&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=65</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:55.994977+09:00</t>
+          <t>2025-08-13T02:16:11.794864+09:00</t>
         </is>
       </c>
     </row>
@@ -2291,25 +2291,25 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>[수분진정] 아비브 어성초 카밍 토너 스킨부스터 더블 기획 (200ml+200ml)</t>
+          <t>[8월 올영픽] 아이오페 레티놀 슈퍼 바운스 세럼 30ml 한정기획 (+20ml+선앰플 20ml)</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>27,300원</t>
+          <t>38,300원</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>27300</v>
+        <v>38300</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000155253&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=66</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000224685&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=66</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:56.040061+09:00</t>
+          <t>2025-08-13T02:16:11.837385+09:00</t>
         </is>
       </c>
     </row>
@@ -2319,25 +2319,25 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>[8월 올영픽] 아이오페 레티놀 슈퍼 바운스 세럼 30ml 한정기획 (+20ml+선앰플 20ml)</t>
+          <t>[테리백증정]해피바스 티트리시카 등드름 케어바디워시 900G</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>38,300원</t>
+          <t>8,900원 ~</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>38300</v>
+        <v>8900</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000224685&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=67</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000202527&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=67</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:56.090615+09:00</t>
+          <t>2025-08-13T02:16:11.882159+09:00</t>
         </is>
       </c>
     </row>
@@ -2347,25 +2347,25 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>플라이밀 단백질쉐이크 45g 9종 택1</t>
+          <t>[1등미백앰플/대용량기획]메디큐브 PDRN 핑크 펩타이드 앰플 30ml 리필기획(본품 30ML+리필 50ML)</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>2,970원 ~</t>
+          <t>25,900원</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>2970</v>
+        <v>25900</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000190168&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=68</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000226498&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=68</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:56.138924+09:00</t>
+          <t>2025-08-13T02:16:11.936269+09:00</t>
         </is>
       </c>
     </row>
@@ -2375,25 +2375,25 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>[올영 어워즈 1등 크림]에스트라 아토베리어365 크림 80ml</t>
+          <t>식물나라 가벼운 수분 선 젤 60ml (단품/2개입)</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>33,000원</t>
+          <t>13,800원 ~</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>33000</v>
+        <v>13800</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000198320&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=69</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000223906&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=69</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:56.188462+09:00</t>
+          <t>2025-08-13T02:16:11.970695+09:00</t>
         </is>
       </c>
     </row>
@@ -2403,25 +2403,25 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>페리페라 스피디 스키니 브로우 7 Colors</t>
+          <t>[8월 올영픽/트러블 1등] 파티온 노스카나인 트러블 세럼 50ml 기획(+15ml+마스크 1매)</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>5,700원 ~</t>
+          <t>26,500원</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>5700</v>
+        <v>26500</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000138671&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=70</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000219717&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=70</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:56.238163+09:00</t>
+          <t>2025-08-13T02:16:12.007044+09:00</t>
         </is>
       </c>
     </row>
@@ -2431,25 +2431,25 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>[8월 올영픽/트러블 1등] 파티온 노스카나인 트러블 세럼 50ml 기획(+15ml+마스크 1매)</t>
+          <t>[수분진정/세럼증정] 닥터지 레드 블레미쉬 클리어 수딩 크림 70ml 증정기획 2종</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>26,500원</t>
+          <t>27,600원 ~</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>26500</v>
+        <v>27600</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000219717&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=71</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000164615&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=71</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:56.278651+09:00</t>
+          <t>2025-08-13T02:16:12.039074+09:00</t>
         </is>
       </c>
     </row>
@@ -2459,25 +2459,25 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>[8월 올영픽/이사배브랜드] 투슬래시포 엔젤릭 새틴 쿠션 기획 (+파우치 증정)</t>
+          <t>[8월 올영픽/대용량] 바이오가 등드름 바디워시 베타인살리실레이트 1000ml</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>37,800원 ~</t>
+          <t>21,160원</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>37800</v>
+        <v>21160</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231020&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=72</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000209207&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=72</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:56.309434+09:00</t>
+          <t>2025-08-13T02:16:12.084750+09:00</t>
         </is>
       </c>
     </row>
@@ -2487,25 +2487,25 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>식물나라 가벼운 수분 선 젤 60ml (단품/2개입)</t>
+          <t>[1위수상] 토리든 마스크 10매 기획 3종 (수분/진정/브라이트닝)</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>13,800원 ~</t>
+          <t>14,500원 ~</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>13800</v>
+        <v>14500</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000223906&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=73</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000158752&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=73</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:56.336357+09:00</t>
+          <t>2025-08-13T02:16:12.128915+09:00</t>
         </is>
       </c>
     </row>
@@ -2515,25 +2515,25 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>[테리백증정]해피바스 티트리시카 등드름 케어바디워시 900G</t>
+          <t>[8월 올영픽/이사배브랜드] 투슬래시포 엔젤릭 새틴 쿠션 기획 (+파우치 증정)</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>8,900원 ~</t>
+          <t>37,800원 ~</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>8900</v>
+        <v>37800</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000202527&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=74</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231020&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=74</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:56.377485+09:00</t>
+          <t>2025-08-13T02:16:12.167552+09:00</t>
         </is>
       </c>
     </row>
@@ -2543,25 +2543,25 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>[8월 올영픽][NEW/단독기획]하트퍼센트 도트 온 무드 립펜슬 0.8g 22종 (기획/단품)</t>
+          <t>[KBO 키링 랜덤 증정] 메디힐 마데카소사이드 수분 선 세럼 흔적 리페어 50g 기획(KBO 에디션)</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>11,900원 ~</t>
+          <t>13,600원 ~</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>11900</v>
+        <v>13600</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000174066&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=75</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231037&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=75</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:56.429566+09:00</t>
+          <t>2025-08-13T02:16:12.207422+09:00</t>
         </is>
       </c>
     </row>
@@ -2571,25 +2571,25 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>[말끔모공/피지순삭] 아누아 어성초 클렌징 듀오 기획 (오일 200ml+폼 150ml)</t>
+          <t>페리페라 스피디 스키니 브로우 7 Colors</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>25,500원</t>
+          <t>5,700원 ~</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>25500</v>
+        <v>5700</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000225774&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=76</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000138671&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=76</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:56.478229+09:00</t>
+          <t>2025-08-13T02:16:12.248968+09:00</t>
         </is>
       </c>
     </row>
@@ -2599,25 +2599,25 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>[8월 올영픽/대용량] 바이오가 등드름 바디워시 베타인살리실레이트 1000ml</t>
+          <t>[8월 올영픽][NEW/단독기획]하트퍼센트 도트 온 무드 립펜슬 0.8g 22종 (기획/단품)</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>21,160원</t>
+          <t>11,900원 ~</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>21160</v>
+        <v>11900</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000209207&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=77</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000174066&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=77</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:56.514014+09:00</t>
+          <t>2025-08-13T02:16:12.287924+09:00</t>
         </is>
       </c>
     </row>
@@ -2627,25 +2627,25 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>[KBO 키링 랜덤 증정] 메디힐 마데카소사이드 수분 선 세럼 흔적 리페어 50g 기획(KBO 에디션)</t>
+          <t>[1등세럼] 브링그린 징크테카 트러블 세럼 기획 50ml 리필기획</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>13,600원 ~</t>
+          <t>29,800원 ~</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>13600</v>
+        <v>29800</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231037&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=78</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000228890&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=78</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:56.566186+09:00</t>
+          <t>2025-08-13T02:16:12.332664+09:00</t>
         </is>
       </c>
     </row>
@@ -2655,25 +2655,25 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>[8/12 하루특가[Y존냄새제거] 바솔 포밍워시 여성청결제 기획(이너밸런싱/마일드캄) 4종 택 1</t>
+          <t>[미니 속광도화밤 증정 기획] 투크 워터프루프 슬림 아이라이너 17colors (기획/단품)</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>17,200원 ~</t>
+          <t>11,900원 ~</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>17200</v>
+        <v>11900</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000204867&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=79</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000185046&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=79</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:56.618902+09:00</t>
+          <t>2025-08-13T02:16:12.367748+09:00</t>
         </is>
       </c>
     </row>
@@ -2683,25 +2683,25 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>[8월 올영픽] 쏘피 쿨링프레쉬 생리대 9종 택 1 (라이너/패드/안심숙면팬티)</t>
+          <t>[올영 어워즈 1등 크림]에스트라 아토베리어365 크림 80ml</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>3,500원 ~</t>
+          <t>33,000원</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>3500</v>
+        <v>33000</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000223283&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=80</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000198320&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=80</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:56.667213+09:00</t>
+          <t>2025-08-13T02:16:12.408402+09:00</t>
         </is>
       </c>
     </row>
@@ -2711,25 +2711,25 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>[8월 올영픽/포켓몬 에디션]성분에디터 실크펩타이드 EGF 하트핏 볼륨 리프팅 앰플 40ml 더블 기획(+키링 파우치)</t>
+          <t>[3년 연속 1위] 콜레올로지 PRO 600mg*30정/60정 (15일/1개월분)</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>25,800원</t>
+          <t>16,900원 ~</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>25800</v>
+        <v>16900</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231076&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=81</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000175634&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=81</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:56.711279+09:00</t>
+          <t>2025-08-13T02:16:12.452556+09:00</t>
         </is>
       </c>
     </row>
@@ -2739,25 +2739,25 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>[미니 속광도화밤 증정 기획] 투크 워터프루프 슬림 아이라이너 17colors (기획/단품)</t>
+          <t>[백태순삭] 라덴스 베럴 혀클리너 (블루/그레이)</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>11,900원 ~</t>
+          <t>8,460원 ~</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>11900</v>
+        <v>8460</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000185046&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=82</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000173609&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=82</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:56.751206+09:00</t>
+          <t>2025-08-13T02:16:12.494718+09:00</t>
         </is>
       </c>
     </row>
@@ -2767,25 +2767,25 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>[1위수상] 토리든 마스크 10매 기획 3종 (수분/진정/브라이트닝)</t>
+          <t>[8/12 하루특가[Y존냄새제거] 바솔 포밍워시 여성청결제 기획(이너밸런싱/마일드캄) 4종 택 1</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>14,500원 ~</t>
+          <t>17,200원 ~</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>14500</v>
+        <v>17200</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000158752&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=83</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000204867&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=83</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:56.795307+09:00</t>
+          <t>2025-08-13T02:16:12.544091+09:00</t>
         </is>
       </c>
     </row>
@@ -2795,25 +2795,25 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>[8월 올영픽] 구달 청귤 비타C 잡티케어 크림 알파 75ml 리필 기획</t>
+          <t>헤라 블랙쿠션 본품15g+리필15g</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>22,300원</t>
+          <t>66,600원 ~</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>22300</v>
+        <v>66600</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230655&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=84</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000202777&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=84</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:56.835927+09:00</t>
+          <t>2025-08-13T02:16:12.589019+09:00</t>
         </is>
       </c>
     </row>
@@ -2841,7 +2841,7 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:56.875197+09:00</t>
+          <t>2025-08-13T02:16:12.643773+09:00</t>
         </is>
       </c>
     </row>
@@ -2851,25 +2851,25 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>[63관왕 No.1] 메디힐 네모패드 100매 8종 피부 고민별 골라담기</t>
+          <t>[증정기획/대용량] 토리든 다이브인 저분자 히알루론산 토너 500ml 기획 (+화장솜 60매 증정)</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>17,500원 ~</t>
+          <t>21,750원</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>17500</v>
+        <v>21750</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000171426&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=86</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000180474&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=86</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:56.922872+09:00</t>
+          <t>2025-08-13T02:16:12.691832+09:00</t>
         </is>
       </c>
     </row>
@@ -2879,25 +2879,25 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>[8월 올영픽/하트거울증정] 이니스프리 비타민C 그린티 엔자임 세럼 30ml 더블 기획</t>
+          <t>[흔적진정] 마몽드 카밍 샷 아줄렌 흔적 수분 앰플 50ml 기획</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>28,220원</t>
+          <t>18,900원 ~</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>28220</v>
+        <v>18900</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230206&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=87</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000219389&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=87</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:56.966119+09:00</t>
+          <t>2025-08-13T02:16:12.737151+09:00</t>
         </is>
       </c>
     </row>
@@ -2907,25 +2907,25 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>[8월올영픽/단독기획] 프리메라 비타티놀 바운시 리프트 세럼 30g+20g 기획</t>
+          <t>[8월올영픽/미니틴트증정] 라카 맥시 글레이어 틴트 3.8g 20종 (단품/기획)</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>31,200원 ~</t>
+          <t>13,500원 ~</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>31200</v>
+        <v>13500</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231293&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=88</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000228370&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=88</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:57.017825+09:00</t>
+          <t>2025-08-13T02:16:12.779863+09:00</t>
         </is>
       </c>
     </row>
@@ -2935,25 +2935,25 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>[8월올영픽/미니틴트증정] 라카 맥시 글레이어 틴트 3.8g 20종 (단품/기획)</t>
+          <t>[8월올영픽/단독기획] 프리메라 비타티놀 바운시 리프트 세럼 30g+20g 기획</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>13,500원 ~</t>
+          <t>31,200원 ~</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>13500</v>
+        <v>31200</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000228370&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=89</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231293&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=89</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:57.060157+09:00</t>
+          <t>2025-08-13T02:16:12.828665+09:00</t>
         </is>
       </c>
     </row>
@@ -2963,25 +2963,25 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>[백태순삭] 라덴스 베럴 혀클리너 (블루/블랙/그레이/화이트)</t>
+          <t>[8월 올영픽/하트거울증정] 이니스프리 비타민C 그린티 엔자임 세럼 30ml 더블 기획</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>8,460원 ~</t>
+          <t>28,220원</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>8460</v>
+        <v>28220</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000159233&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=90</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230206&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=90</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:57.092958+09:00</t>
+          <t>2025-08-13T02:16:12.856311+09:00</t>
         </is>
       </c>
     </row>
@@ -2991,25 +2991,25 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>[증정기획/대용량] 토리든 다이브인 저분자 히알루론산 토너 500ml 기획 (+화장솜 60매 증정)</t>
+          <t>[진정커버/1위쿠션] 파넬 시카마누 세럼쿠션(본품+리필)</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>21,750원</t>
+          <t>27,750원 ~</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>21750</v>
+        <v>27750</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000180474&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=91</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000190611&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=91</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:57.122578+09:00</t>
+          <t>2025-08-13T02:16:12.906299+09:00</t>
         </is>
       </c>
     </row>
@@ -3019,25 +3019,25 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>[1등세럼] 브링그린 징크테카 트러블 세럼 기획 50ml 리필기획</t>
+          <t>[말끔모공/피지순삭] 아누아 어성초 클렌징 듀오 기획 (오일 200ml+폼 150ml)</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>29,800원 ~</t>
+          <t>25,500원</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>29800</v>
+        <v>25500</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000228890&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=92</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000225774&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=92</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:57.145922+09:00</t>
+          <t>2025-08-13T02:16:12.946550+09:00</t>
         </is>
       </c>
     </row>
@@ -3047,25 +3047,25 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>[8월 올영픽/국동호PICK/쿨링진정] 에스네이처 아쿠아 오아시스 수분 젤크림 90ml 기획 (+카밍패드 2매)</t>
+          <t>[8월 올영픽/포켓몬 에디션]성분에디터 실크펩타이드 EGF 하트핏 볼륨 리프팅 앰플 40ml 더블 기획(+키링 파우치)</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>21,900원</t>
+          <t>25,800원</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>21900</v>
+        <v>25800</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000202893&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=93</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231076&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=93</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:57.192625+09:00</t>
+          <t>2025-08-13T02:16:12.989758+09:00</t>
         </is>
       </c>
     </row>
@@ -3075,25 +3075,25 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>[진정커버/1위쿠션] 파넬 시카마누 세럼쿠션(본품+리필)</t>
+          <t>[백태순삭] 라덴스 베럴 혀클리너 (블루/블랙/그레이/화이트)</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>27,750원 ~</t>
+          <t>8,460원 ~</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>27750</v>
+        <v>8460</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000190611&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=94</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000159233&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=94</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:57.240699+09:00</t>
+          <t>2025-08-13T02:16:13.041987+09:00</t>
         </is>
       </c>
     </row>
@@ -3103,25 +3103,25 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>[화잘먹] 구달 맑은 어성초 진정 수분 선크림 50ml 1+1 기획</t>
+          <t>[8월 올영픽] 구달 청귤 비타C 잡티케어 크림 알파 75ml 리필 기획</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>16,500원 ~</t>
+          <t>22,300원</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>16500</v>
+        <v>22300</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000219553&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=95</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230655&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=95</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:57.293206+09:00</t>
+          <t>2025-08-13T02:16:13.099610+09:00</t>
         </is>
       </c>
     </row>
@@ -3131,25 +3131,25 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>[8월 올영픽/핑구콜라보] 코스노리 아이래쉬 틴팅 세럼 비건 블랙 속눈썹영양제 (단품/기획)</t>
+          <t>아디다스 EDP 30ml/50ml/100ml 6종 택 1</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>14,400원 ~</t>
+          <t>20,200원 ~</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>14400</v>
+        <v>20200</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000187890&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=96</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230142&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=96</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:57.337886+09:00</t>
+          <t>2025-08-13T02:16:13.137742+09:00</t>
         </is>
       </c>
     </row>
@@ -3159,25 +3159,25 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>[백태순삭] 라덴스 베럴 혀클리너 (블루/그레이)</t>
+          <t>[8월 올영픽] 쏘피 쿨링프레쉬 생리대 9종 택 1 (라이너/패드/안심숙면팬티)</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>8,460원 ~</t>
+          <t>3,500원 ~</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>8460</v>
+        <v>3500</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000173609&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=97</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000223283&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=97</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:57.385130+09:00</t>
+          <t>2025-08-13T02:16:13.165880+09:00</t>
         </is>
       </c>
     </row>
@@ -3187,25 +3187,25 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>[핑거모공브러시증정] 한율 쑥시카 쑥떡 팩폼 120ml 기획 (+15ml 미니어처)</t>
+          <t>[8월 올영픽/핑구콜라보] 코스노리 아이래쉬 틴팅 세럼 비건 블랙 속눈썹영양제 (단품/기획)</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>19,800원</t>
+          <t>14,400원 ~</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>19800</v>
+        <v>14400</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000204014&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=98</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000187890&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=98</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:57.436720+09:00</t>
+          <t>2025-08-13T02:16:13.190319+09:00</t>
         </is>
       </c>
     </row>
@@ -3215,25 +3215,25 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>[올영단독/10+1] 메디힐 마데카소사이드 에센셜 마스크 흔적 리페어 10+1매 기획</t>
+          <t>[단독/추가증정] 1+1 려 루트젠 탈모증상케어 두피에센스 80ml 더블기획+샴푸50ml</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>10,000원</t>
+          <t>21,900원 ~</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>10000</v>
+        <v>21900</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000209520&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=99</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000197603&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=99</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:57.493456+09:00</t>
+          <t>2025-08-13T02:16:13.224008+09:00</t>
         </is>
       </c>
     </row>
@@ -3243,25 +3243,25 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>[신상출시] 딜라이트 프로젝트 곤약워터젤리 단품/10개입 12종 택1</t>
+          <t>[화잘먹] 구달 맑은 어성초 진정 수분 선크림 50ml 1+1 기획</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>1,710원 ~</t>
+          <t>16,500원 ~</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>1710</v>
+        <v>16500</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000209365&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=100</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000219553&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=100</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>2025-08-13T01:55:57.531219+09:00</t>
+          <t>2025-08-13T02:16:13.255780+09:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update scraper workflow and OliveYoung rankings data
Co-authored-by: jongpard <jongpard@gmail.com>
</commit_message>
<xml_diff>
--- a/oliveyoung_rankings_2025-08-13.xlsx
+++ b/oliveyoung_rankings_2025-08-13.xlsx
@@ -489,7 +489,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:09.334730+09:00</t>
+          <t>2025-08-13T02:52:59.456184+09:00</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:09.381622+09:00</t>
+          <t>2025-08-13T02:52:59.476164+09:00</t>
         </is>
       </c>
     </row>
@@ -527,25 +527,25 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[쓰까르3일마켓] [리뷰이벤트/크림본품증정] 메디큐브 에이지알 부스터프로 미니플러스 베이지/핑크</t>
+          <t>쏘내추럴 올 데이 메이크업 픽서 더블기획 (120ml+120ml)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>107,500원 ~</t>
+          <t>29,930원</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>107500</v>
+        <v>29930</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231154&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=3</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000162114&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=3</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:09.422530+09:00</t>
+          <t>2025-08-13T02:52:59.515825+09:00</t>
         </is>
       </c>
     </row>
@@ -555,25 +555,25 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>쏘내추럴 올 데이 메이크업 픽서 더블기획 (120ml+120ml)</t>
+          <t>[쓰까르3일마켓] [리뷰이벤트/크림본품증정] 메디큐브 에이지알 부스터프로 미니플러스 베이지/핑크</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>29,930원</t>
+          <t>107,500원 ~</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>29930</v>
+        <v>107500</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000162114&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=4</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231154&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=4</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:09.458947+09:00</t>
+          <t>2025-08-13T02:52:59.572476+09:00</t>
         </is>
       </c>
     </row>
@@ -601,7 +601,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:09.504142+09:00</t>
+          <t>2025-08-13T02:52:59.626045+09:00</t>
         </is>
       </c>
     </row>
@@ -629,7 +629,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:09.539674+09:00</t>
+          <t>2025-08-13T02:52:59.675988+09:00</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:09.592912+09:00</t>
+          <t>2025-08-13T02:52:59.730689+09:00</t>
         </is>
       </c>
     </row>
@@ -685,7 +685,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:09.642444+09:00</t>
+          <t>2025-08-13T02:52:59.783883+09:00</t>
         </is>
       </c>
     </row>
@@ -695,25 +695,25 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[고민영PICK/한정기획] 아벤느 이드랑스 에센스 인 로션 200ml 한정 기획 (+100ml*2) *수분 충전</t>
+          <t>[천만돌파/1+1] 비플레인 녹두 약산성 클렌징폼 160ml+160ml 기획</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>27,900원</t>
+          <t>23,500원</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>27900</v>
+        <v>23500</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230424&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=9</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000222605&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=9</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:09.691991+09:00</t>
+          <t>2025-08-13T02:52:59.834378+09:00</t>
         </is>
       </c>
     </row>
@@ -723,25 +723,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[천만돌파/1+1] 비플레인 녹두 약산성 클렌징폼 160ml+160ml 기획</t>
+          <t>[8월 펀딩][당0g대] 크런틴 크런치볼 단백질쉐이크 초코이즈백 3box(15팩)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>23,500원</t>
+          <t>57,900원</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>23500</v>
+        <v>57900</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000222605&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=10</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=B000000227402&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=10</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:09.732831+09:00</t>
+          <t>2025-08-13T02:52:59.876960+09:00</t>
         </is>
       </c>
     </row>
@@ -751,25 +751,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[8월 펀딩][당0g대] 크런틴 크런치볼 단백질쉐이크 초코이즈백 3box(15팩)</t>
+          <t>[7일특가/좌두pick] 마미케어 바다포도 모공앰플 50ml</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>57,900원</t>
+          <t>13,800원</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>57900</v>
+        <v>13800</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=B000000227402&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=11</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000224295&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=11</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:09.750559+09:00</t>
+          <t>2025-08-13T02:52:59.924534+09:00</t>
         </is>
       </c>
     </row>
@@ -779,25 +779,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[푸디젠 PICK | 리뷰 이벤트] 구달 청귤 비타C 잡티케어 세럼 알파 50ml 리필 기획 (+크림 10ml)</t>
+          <t>[NEW] 아누아 TXA 나이아신 흔적 세럼 30ml 2입</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>28,500원</t>
+          <t>27,500원</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>28500</v>
+        <v>27500</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230654&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=12</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000226201&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=12</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:09.765067+09:00</t>
+          <t>2025-08-13T02:52:59.974051+09:00</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:09.781720+09:00</t>
+          <t>2025-08-13T02:53:00.024119+09:00</t>
         </is>
       </c>
     </row>
@@ -835,25 +835,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[8월 올영픽/NO.1 미스트세럼] 달바 퍼스트 스프레이 세럼 100ml 2개 기획</t>
+          <t>[푸디젠 PICK | 리뷰 이벤트] 구달 청귤 비타C 잡티케어 세럼 알파 50ml 리필 기획 (+크림 10ml)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>32,900원</t>
+          <t>28,500원</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>32900</v>
+        <v>28500</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000179685&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=14</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230654&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=14</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:09.804461+09:00</t>
+          <t>2025-08-13T02:53:00.073743+09:00</t>
         </is>
       </c>
     </row>
@@ -863,25 +863,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[7일특가/좌두pick] 마미케어 바다포도 모공앰플 50ml</t>
+          <t>[8월 올영픽/NO.1 미스트세럼] 달바 퍼스트 스프레이 세럼 100ml 2개 기획</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>13,800원</t>
+          <t>32,900원</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>13800</v>
+        <v>32900</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000224295&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=15</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000179685&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=15</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:09.841858+09:00</t>
+          <t>2025-08-13T02:53:00.114994+09:00</t>
         </is>
       </c>
     </row>
@@ -891,25 +891,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[NEW] 아누아 TXA 나이아신 흔적 세럼 30ml 2입</t>
+          <t>[3시간팩] 바이오던스 리얼 딥 마스크 7매 (콜라겐, 세라놀, 비타, 씨켈프)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>27,500원</t>
+          <t>28,900원 ~</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>27500</v>
+        <v>28900</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000226201&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=16</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000221807&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=16</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:09.891196+09:00</t>
+          <t>2025-08-13T02:53:00.166350+09:00</t>
         </is>
       </c>
     </row>
@@ -919,25 +919,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[3시간팩] 바이오던스 리얼 딥 마스크 7매 (콜라겐, 세라놀, 비타, 씨켈프)</t>
+          <t>[꼬마마법사 레미 콜라보/100% 리뷰이벤트] 키스미 아이 블러 이펙트 틴트 3.5g 7종 (올영 단독 선론칭)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>28,900원 ~</t>
+          <t>12,900원 ~</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>28900</v>
+        <v>12900</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000221807&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=17</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000214282&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=17</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:09.936987+09:00</t>
+          <t>2025-08-13T02:53:00.208007+09:00</t>
         </is>
       </c>
     </row>
@@ -947,25 +947,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[4년연속1위/블랙헤드OUT] 마녀공장 퓨어 클렌징 오일 300ml 기획 (+25mlx2)</t>
+          <t>[8월올영픽] 아비브 어성초 흔적 에센스 패드 클리어터치 140매 (70매+70매 리필)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>19,900원</t>
+          <t>26,600원</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>19900</v>
+        <v>26600</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000199588&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=18</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000219555&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=18</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:09.982056+09:00</t>
+          <t>2025-08-13T02:53:00.255426+09:00</t>
         </is>
       </c>
     </row>
@@ -975,25 +975,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>[꼬마마법사 레미 콜라보/100% 리뷰이벤트] 키스미 아이 블러 이펙트 틴트 3.5g 7종 (올영 단독 선론칭)</t>
+          <t>[4년연속1위/블랙헤드OUT] 마녀공장 퓨어 클렌징 오일 300ml 기획 (+25mlx2)</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>12,900원 ~</t>
+          <t>19,900원</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>12900</v>
+        <v>19900</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000214282&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=19</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000199588&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=19</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:10.032620+09:00</t>
+          <t>2025-08-13T02:53:00.301346+09:00</t>
         </is>
       </c>
     </row>
@@ -1003,25 +1003,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[시드니픽/8월] 아벤느 클리낭스 클렌징젤 400ml 더블기획 (클리낭스 세럼 2ml + 클리낭스아쿠아크림인젤 2ml)</t>
+          <t>세노비스 밀크씨슬 120캡슐 (4개월분)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>28,900원</t>
+          <t>25,000원</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>28900</v>
+        <v>25000</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230423&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=20</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000129053&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=20</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:10.079682+09:00</t>
+          <t>2025-08-13T02:53:00.345878+09:00</t>
         </is>
       </c>
     </row>
@@ -1031,25 +1031,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>[8월올영픽] 아비브 어성초 흔적 에센스 패드 클리어터치 140매 (70매+70매 리필)</t>
+          <t>[NEW] 브링그린 티트리시카수딩크림플러스100ml (단품/2입)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>26,600원</t>
+          <t>19,800원 ~</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>26600</v>
+        <v>19800</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000219555&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=21</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000226553&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=21</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:10.125703+09:00</t>
+          <t>2025-08-13T02:53:00.389510+09:00</t>
         </is>
       </c>
     </row>
@@ -1059,25 +1059,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>[3년 연속 1위] 어노브 딥 데미지 헤어 트리트먼트 EX 320ml 더블/듀오 기획 3종 택1</t>
+          <t>[리뷰 이벤트] [아름송이 PICK] 릴리이브 그로우턴 탈모 브러쉬 앰플 100ml 기획 (+100ml 리필 증정)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>29,800원 ~</t>
+          <t>39,800원</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>29800</v>
+        <v>39800</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000171423&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=22</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000218845&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=22</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:10.169112+09:00</t>
+          <t>2025-08-13T02:53:00.440629+09:00</t>
         </is>
       </c>
     </row>
@@ -1087,25 +1087,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>[피지클렌징] 마몽드 어메이징 딥 민트 클렌징밤 90ml 기획 (+폼 30ml)</t>
+          <t>[8월 올영픽/하트거울증정] 이니스프리 레티놀 시카 흔적 앰플 30ml 더블 기획</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16,000원</t>
+          <t>28,710원</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>16000</v>
+        <v>28710</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000198831&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=23</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230208&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=23</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:10.222219+09:00</t>
+          <t>2025-08-13T02:53:00.487254+09:00</t>
         </is>
       </c>
     </row>
@@ -1115,25 +1115,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>아벤느 오 떼르말 미스트 300ml*2 + 50ml 기획</t>
+          <t>라로슈포제 시카플라스트 밤 B5+ 100ml 기획 (+히알루 B5 세럼 1.5ml*2 증정)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>27,900원</t>
+          <t>36,000원</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>27900</v>
+        <v>36000</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000166436&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=24</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000226997&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=24</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:10.272661+09:00</t>
+          <t>2025-08-13T02:53:00.536884+09:00</t>
         </is>
       </c>
     </row>
@@ -1143,25 +1143,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>[리뷰 이벤트] [아름송이 PICK] 릴리이브 그로우턴 탈모 브러쉬 앰플 100ml 기획 (+100ml 리필 증정)</t>
+          <t>[피지클렌징] 마몽드 어메이징 딥 민트 클렌징밤 90ml 기획 (+폼 30ml)</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>39,800원</t>
+          <t>16,000원</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>39800</v>
+        <v>16000</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000218845&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=25</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000198831&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=25</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:10.319028+09:00</t>
+          <t>2025-08-13T02:53:00.578683+09:00</t>
         </is>
       </c>
     </row>
@@ -1171,25 +1171,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>라로슈포제 시카플라스트 밤 B5+ 100ml 기획 (+히알루 B5 세럼 1.5ml*2 증정)</t>
+          <t>[덱스 PICK] 오브제 내추럴 커버 로션 50g 단품/기획(+미니어처 10ml)</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>36,000원</t>
+          <t>26,510원 ~</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>36000</v>
+        <v>26510</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000226997&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=26</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000204975&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=26</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:10.354521+09:00</t>
+          <t>2025-08-13T02:53:00.598661+09:00</t>
         </is>
       </c>
     </row>
@@ -1199,25 +1199,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>세노비스 밀크씨슬 120캡슐 (4개월분)</t>
+          <t>[3년 연속 1위] 어노브 딥 데미지 헤어 트리트먼트 EX 320ml 더블/듀오 기획 3종 택1</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>25,000원</t>
+          <t>29,800원 ~</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>25000</v>
+        <v>29800</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000129053&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=27</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000171423&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=27</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:10.409064+09:00</t>
+          <t>2025-08-13T02:53:00.620495+09:00</t>
         </is>
       </c>
     </row>
@@ -1227,25 +1227,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>[NEW] 브링그린 티트리시카수딩크림플러스100ml (단품/2입)</t>
+          <t>[14년연속 1위] 메디힐 에센셜 마스크팩 1매 고기능 7종 택1</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>19,800원 ~</t>
+          <t>1,000원 ~</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>19800</v>
+        <v>1000</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000226553&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=28</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000217620&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=28</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:10.466378+09:00</t>
+          <t>2025-08-13T02:53:00.671342+09:00</t>
         </is>
       </c>
     </row>
@@ -1255,25 +1255,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>[8월 올영픽/하트거울증정] 이니스프리 레티놀 시카 흔적 앰플 30ml 더블 기획</t>
+          <t>수이사이 뷰티 클리어 파우더워시 산리오 콜라보 6종 택1</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>28,710원</t>
+          <t>19,440원 ~</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>28710</v>
+        <v>19440</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230208&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=29</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230670&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=29</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:10.518220+09:00</t>
+          <t>2025-08-13T02:53:00.705202+09:00</t>
         </is>
       </c>
     </row>
@@ -1283,25 +1283,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>[14년연속 1위] 메디힐 에센셜 마스크팩 1매 고기능 7종 택1</t>
+          <t>[1+1 더블기획] 라곰 셀럽 마이크로 수분 폼 클렌저 120ml x 2</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1,000원 ~</t>
+          <t>24,650원</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>1000</v>
+        <v>24650</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000217620&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=30</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230821&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=30</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:10.555343+09:00</t>
+          <t>2025-08-13T02:53:00.760663+09:00</t>
         </is>
       </c>
     </row>
@@ -1311,25 +1311,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>[1+1 더블기획] 라곰 셀럽 마이크로 수분 폼 클렌저 120ml x 2</t>
+          <t>[단독특가] 푸드올로지 지중해 레몬버베나 500mg 60정 (1개월분)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>24,650원</t>
+          <t>38,100원</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>24650</v>
+        <v>38100</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230821&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=31</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230972&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=31</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:10.604213+09:00</t>
+          <t>2025-08-13T02:53:00.811933+09:00</t>
         </is>
       </c>
     </row>
@@ -1339,25 +1339,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>[KBO 파우치 증정] 메디힐 네모패드 더블기획 3종 골라담기(마데카소사이드, PDRN, 티트리)(KBO 에디션)</t>
+          <t>[8월올영픽/Oiad x 어프어프 콜라보] 오아드 립티크 9종 단품/기획</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>28,900원 ~</t>
+          <t>21,900원 ~</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>28900</v>
+        <v>21900</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231048&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=32</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000218834&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=32</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:10.659729+09:00</t>
+          <t>2025-08-13T02:53:00.864261+09:00</t>
         </is>
       </c>
     </row>
@@ -1367,25 +1367,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>[8월올영픽/Oiad x 어프어프 콜라보] 오아드 립티크 9종 단품/기획</t>
+          <t>[1+1/단독기획] 메디힐 마데카소사이드 흔적 리페어 세럼 40+40ml 더블 기획</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>21,900원 ~</t>
+          <t>22,900원</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>21900</v>
+        <v>22900</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000218834&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=33</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000211119&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=33</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:10.711872+09:00</t>
+          <t>2025-08-13T02:53:00.914942+09:00</t>
         </is>
       </c>
     </row>
@@ -1395,25 +1395,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>[덱스 PICK] 오브제 내추럴 커버 로션 50g 단품/기획(+미니어처 10ml)</t>
+          <t>[KBO 파우치 증정] 메디힐 네모패드 더블기획 3종 골라담기(마데카소사이드, PDRN, 티트리)(KBO 에디션)</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>26,510원 ~</t>
+          <t>28,900원 ~</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>26510</v>
+        <v>28900</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000204975&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=34</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231048&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=34</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:10.750968+09:00</t>
+          <t>2025-08-13T02:53:00.960871+09:00</t>
         </is>
       </c>
     </row>
@@ -1423,25 +1423,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>[단독특가] 푸드올로지 지중해 레몬버베나 500mg 60정 (1개월분)</t>
+          <t>[8월 올영픽/가나디콜라보] 토리든 다이브인 저분자 히알루론산 수딩 크림 100ml 가나디 더블 기획 (+파우치 키링)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>38,100원</t>
+          <t>30,000원</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>38100</v>
+        <v>30000</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230972&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=35</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230832&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=35</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:10.769486+09:00</t>
+          <t>2025-08-13T02:53:00.981243+09:00</t>
         </is>
       </c>
     </row>
@@ -1451,25 +1451,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>[8월 올영픽/가나디콜라보] 토리든 다이브인 저분자 히알루론산 수딩 크림 100ml 가나디 더블 기획 (+파우치 키링)</t>
+          <t>[율리 PICK/5+1매 한정기획] 아이오페 레티놀 세럼 인 겔 마스크 기획</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>30,000원</t>
+          <t>23,600원</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>30000</v>
+        <v>23600</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230832&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=36</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000224510&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=36</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:10.786956+09:00</t>
+          <t>2025-08-13T02:53:00.998545+09:00</t>
         </is>
       </c>
     </row>
@@ -1479,25 +1479,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>[1+1/단독기획] 메디힐 마데카소사이드 흔적 리페어 세럼 40+40ml 더블 기획</t>
+          <t>[NEW/리뉴얼] 컬러그램 누디 블러 틴트 18 COLOR</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>22,900원</t>
+          <t>8,300원 ~</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>22900</v>
+        <v>8300</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000211119&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=37</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230581&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=37</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:10.820134+09:00</t>
+          <t>2025-08-13T02:53:01.019619+09:00</t>
         </is>
       </c>
     </row>
@@ -1507,25 +1507,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>[율리 PICK/5+1매 한정기획] 아이오페 레티놀 세럼 인 겔 마스크 기획</t>
+          <t>바이오더마 시카비오 포마드 100ml(리페어 리치 밤)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>23,600원</t>
+          <t>28,500원</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>23600</v>
+        <v>28500</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000224510&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=38</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000134691&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=38</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:10.867848+09:00</t>
+          <t>2025-08-13T02:53:01.063726+09:00</t>
         </is>
       </c>
     </row>
@@ -1535,25 +1535,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>[8월 올영픽/핑구콜라보] 코스노리 화이트닝 드레스 비건 톤업크림 (단품/기획)</t>
+          <t>[25ml 추가증정] 휩드 비건 팩클렌저 130g 기획 3종 (머그트리/무화버터/유자몽)</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>16,000원 ~</t>
+          <t>19,700원 ~</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>16000</v>
+        <v>19700</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000017135&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=39</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000217511&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=39</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:10.908556+09:00</t>
+          <t>2025-08-13T02:53:01.107768+09:00</t>
         </is>
       </c>
     </row>
@@ -1563,25 +1563,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>수이사이 뷰티 클리어 파우더워시 산리오 콜라보 6종 택1</t>
+          <t>[파격특가] 피지오겔 시카밸런스 포맨 카밍 크림 70ml</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>19,440원 ~</t>
+          <t>9,900원</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>19440</v>
+        <v>9900</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230670&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=40</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000211188&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=40</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:10.939302+09:00</t>
+          <t>2025-08-13T02:53:01.164049+09:00</t>
         </is>
       </c>
     </row>
@@ -1591,25 +1591,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>[NEW/리뉴얼] 컬러그램 누디 블러 틴트 18 COLOR</t>
+          <t>[1+1한정기획/열감진정] 스킨푸드 캐롯 카로틴 카밍 워터 패드 60매 더블기획 (본품+본품)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>8,300원 ~</t>
+          <t>26,900원</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>8300</v>
+        <v>26900</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230581&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=41</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000224932&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=41</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:10.977652+09:00</t>
+          <t>2025-08-13T02:53:01.219256+09:00</t>
         </is>
       </c>
     </row>
@@ -1619,25 +1619,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>[25ml 추가증정] 휩드 비건 팩클렌저 130g 기획 3종 (머그트리/무화버터/유자몽)</t>
+          <t>포뷰트 두피 타투15g 블랙 (+추영우 포토카드 증정 이벤트)</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>19,700원 ~</t>
+          <t>16,800원</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>19700</v>
+        <v>16800</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000217511&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=42</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000223552&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=42</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.030158+09:00</t>
+          <t>2025-08-13T02:53:01.270763+09:00</t>
         </is>
       </c>
     </row>
@@ -1647,25 +1647,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>[1+1한정기획/열감진정] 스킨푸드 캐롯 카로틴 카밍 워터 패드 60매 더블기획 (본품+본품)</t>
+          <t>[3년연속1등] 라보에이치 두피강화샴푸 750+125ML(단품/기획)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>26,900원</t>
+          <t>25,900원 ~</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>26900</v>
+        <v>25900</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000224932&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=43</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000149501&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=43</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.067455+09:00</t>
+          <t>2025-08-13T02:53:01.310177+09:00</t>
         </is>
       </c>
     </row>
@@ -1675,25 +1675,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>[뷰티디바이스 1위] [광채토닝 메디큐브 부스터프로 쿠로미 에디션(+쿠로미헤드캡+세안밴드+디바이스클리너+스티커2종)</t>
+          <t>바이오더마 센시비오 H2O 850ml(클렌징워터)</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>349,000원</t>
+          <t>24,610원</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>349000</v>
+        <v>24610</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000224654&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=44</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000130319&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=44</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.105379+09:00</t>
+          <t>2025-08-13T02:53:01.361551+09:00</t>
         </is>
       </c>
     </row>
@@ -1703,25 +1703,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>바이오더마 시카비오 포마드 100ml(리페어 리치 밤)</t>
+          <t>[산리오캐릭터즈] 롬앤 더 쥬시 래스팅 틴트 (+쉐이킹키링증정) 단품/기획</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>28,500원</t>
+          <t>13,000원 ~</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>28500</v>
+        <v>13000</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000134691&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=45</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000213153&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=45</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.132373+09:00</t>
+          <t>2025-08-13T02:53:01.409247+09:00</t>
         </is>
       </c>
     </row>
@@ -1731,25 +1731,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>[파격특가] 질레트 랩스 딥클렌징바 면도기 (핸들+1입날)</t>
+          <t>[올영픽/피지아웃/화잘먹 수분천재세럼] 에스네이처 아쿠아 스쿠알란 세럼 50ml 기획(+50ml 리필+수분크림10ml)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>9,900원</t>
+          <t>21,700원</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>9900</v>
+        <v>21700</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000174122&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=46</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000188004&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=46</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.157314+09:00</t>
+          <t>2025-08-13T02:53:01.461760+09:00</t>
         </is>
       </c>
     </row>
@@ -1759,25 +1759,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>[파격특가] 피지오겔 시카밸런스 포맨 카밍 크림 70ml</t>
+          <t>[유시은pick/1등홈경락템] 마미케어 EMS브이쎄라 (화이트/핑크/NEW 퍼플에디션) (+전용 부스팅젤 본품 증정)</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>9,900원</t>
+          <t>99,000원 ~</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>9900</v>
+        <v>99000</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000211188&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=47</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=B000000224350&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=47</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.175181+09:00</t>
+          <t>2025-08-13T02:53:01.505969+09:00</t>
         </is>
       </c>
     </row>
@@ -1787,25 +1787,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>바이오더마 센시비오 H2O 850ml(클렌징워터)</t>
+          <t>[8월 올영픽]오브제 포어 제로 오일 컨트롤 선스틱 18g</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>24,610원</t>
+          <t>17,800원</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>24610</v>
+        <v>17800</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000130319&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=48</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000225044&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=48</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.193860+09:00</t>
+          <t>2025-08-13T02:53:01.564129+09:00</t>
         </is>
       </c>
     </row>
@@ -1815,25 +1815,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>[산리오캐릭터즈] 롬앤 더 쥬시 래스팅 틴트 (+쉐이킹키링증정) 단품/기획</t>
+          <t>플라이밀 단백질쉐이크 45g 9종 택1</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>13,000원 ~</t>
+          <t>2,970원 ~</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>13000</v>
+        <v>2970</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000213153&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=49</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000190168&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=49</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.224068+09:00</t>
+          <t>2025-08-13T02:53:01.617090+09:00</t>
         </is>
       </c>
     </row>
@@ -1843,25 +1843,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>[3년연속1등] 라보에이치 두피강화샴푸 750+125ML(단품/기획)</t>
+          <t>[1등 속눈썹/NEW] 코링코 톡톡하라 노글루 속눈썹 11종 택1</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>25,900원 ~</t>
+          <t>13,900원 ~</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>25900</v>
+        <v>13900</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000149501&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=50</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000213569&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=50</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.268140+09:00</t>
+          <t>2025-08-13T02:53:01.665488+09:00</t>
         </is>
       </c>
     </row>
@@ -1871,25 +1871,25 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>[유시은pick/1등홈경락템] 마미케어 EMS브이쎄라 (화이트/핑크/NEW 퍼플에디션) (+전용 부스팅젤 본품 증정)</t>
+          <t>[NEW/8월올영픽] 플르부아 디퓨저 200ml &amp; 센티드 타블렛(퍼퓸 샤쉐) 단품/기획</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>99,000원 ~</t>
+          <t>26,300원 ~</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>99000</v>
+        <v>26300</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=B000000224350&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=51</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000202553&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=51</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.314313+09:00</t>
+          <t>2025-08-13T02:53:01.708065+09:00</t>
         </is>
       </c>
     </row>
@@ -1899,25 +1899,25 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>[8월 올영픽]오브제 포어 제로 오일 컨트롤 선스틱 18g</t>
+          <t>[파격특가] 질레트 랩스 딥클렌징바 면도기 (핸들+1입날)</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>17,800원</t>
+          <t>9,900원</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>17800</v>
+        <v>9900</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000225044&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=52</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000174122&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=52</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.356490+09:00</t>
+          <t>2025-08-13T02:53:01.753553+09:00</t>
         </is>
       </c>
     </row>
@@ -1927,25 +1927,25 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>[1등 속눈썹/NEW] 코링코 톡톡하라 노글루 속눈썹 11종 택1</t>
+          <t>[8월 올영픽/핑구콜라보] 코스노리 화이트닝 드레스 비건 톤업크림 (단품/기획)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>13,900원 ~</t>
+          <t>16,000원 ~</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>13900</v>
+        <v>16000</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000213569&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=53</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000017135&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=53</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.387148+09:00</t>
+          <t>2025-08-13T02:53:01.789832+09:00</t>
         </is>
       </c>
     </row>
@@ -1955,25 +1955,25 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>포뷰트 두피 타투15g 블랙 (+추영우 포토카드 증정 이벤트)</t>
+          <t>[1등진정/크라이베이비 이벤트] 파넬 시카마누 92세럼 더블기획(30ml+30ml)</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16,800원</t>
+          <t>22,900원</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>16800</v>
+        <v>22900</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000223552&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=54</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000189713&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=54</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.433238+09:00</t>
+          <t>2025-08-13T02:53:01.824732+09:00</t>
         </is>
       </c>
     </row>
@@ -1983,25 +1983,25 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>[올영픽/피지아웃/화잘먹 수분천재세럼] 에스네이처 아쿠아 스쿠알란 세럼 50ml 기획(+50ml 리필+수분크림10ml)</t>
+          <t>[8월올영픽/포켓몬 에디션]성분에디터 그린토마토 NMN 포어 리프팅 앰플 40ml 더블 기획 (+키링 파우치)</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>21,700원</t>
+          <t>22,800원</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>21700</v>
+        <v>22800</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000188004&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=55</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230914&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=55</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.476543+09:00</t>
+          <t>2025-08-13T02:53:01.877217+09:00</t>
         </is>
       </c>
     </row>
@@ -2011,25 +2011,25 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>[8월 올영픽] [유시몰X헌터] 장화스탠더+퍼플코렉터 미백치약 106g*2</t>
+          <t>식물나라 가벼운 수분 선 젤 60ml (단품/2개입)</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>25,900원</t>
+          <t>13,800원 ~</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>25900</v>
+        <v>13800</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230647&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=56</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000223906&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=56</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.511086+09:00</t>
+          <t>2025-08-13T02:53:01.927796+09:00</t>
         </is>
       </c>
     </row>
@@ -2039,25 +2039,25 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>[NEW/8월올영픽] 플르부아 디퓨저 200ml &amp; 센티드 타블렛(퍼퓸 샤쉐) 단품/기획</t>
+          <t>[태닝포차코/한정] 바이탈뷰티 메타그린 슬림업 60정 기획 (+포차코 파우치 증정)</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>26,300원 ~</t>
+          <t>28,320원</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>26300</v>
+        <v>28320</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000202553&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=57</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000229143&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=57</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.545366+09:00</t>
+          <t>2025-08-13T02:53:01.980189+09:00</t>
         </is>
       </c>
     </row>
@@ -2067,25 +2067,25 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>[8월올영픽/포켓몬 에디션]성분에디터 그린토마토 NMN 포어 리프팅 앰플 40ml 더블 기획 (+키링 파우치)</t>
+          <t>[수분진정] 아비브 어성초 카밍 토너 스킨부스터 더블 기획 (200ml+200ml)</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>22,800원</t>
+          <t>27,300원</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>22800</v>
+        <v>27300</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230914&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=58</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000155253&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=58</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.565847+09:00</t>
+          <t>2025-08-13T02:53:02.029950+09:00</t>
         </is>
       </c>
     </row>
@@ -2095,25 +2095,25 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>[1등진정/크라이베이비 이벤트] 파넬 시카마누 92세럼 더블기획(30ml+30ml)</t>
+          <t>[한겹밀착커버] 에이프릴스킨 히어로쿠션 핑크에디션(본품+리필+퍼프2개)</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>22,900원</t>
+          <t>24,900원 ~</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>22900</v>
+        <v>24900</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000189713&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=59</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000163765&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=59</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.582181+09:00</t>
+          <t>2025-08-13T02:53:02.085246+09:00</t>
         </is>
       </c>
     </row>
@@ -2123,25 +2123,25 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>[태닝포차코/한정] 바이탈뷰티 메타그린 슬림업 60정 기획 (+포차코 파우치 증정)</t>
+          <t>[8월 올영픽] 아이오페 레티놀 슈퍼 바운스 세럼 30ml 한정기획 (+20ml+선앰플 20ml)</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>28,320원</t>
+          <t>38,300원</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>28320</v>
+        <v>38300</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000229143&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=60</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000224685&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=60</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.604781+09:00</t>
+          <t>2025-08-13T02:53:02.125603+09:00</t>
         </is>
       </c>
     </row>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.645656+09:00</t>
+          <t>2025-08-13T02:53:02.179292+09:00</t>
         </is>
       </c>
     </row>
@@ -2179,25 +2179,25 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>[한겹밀착커버] 에이프릴스킨 히어로쿠션 핑크에디션(본품+리필+퍼프2개)</t>
+          <t>[고민영PICK/한정기획] 아벤느 이드랑스 에센스 인 로션 200ml 한정 기획 (+100ml*2) *수분 충전</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>24,900원 ~</t>
+          <t>27,900원</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>24900</v>
+        <v>27900</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000163765&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=62</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230424&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=62</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.681822+09:00</t>
+          <t>2025-08-13T02:53:02.232079+09:00</t>
         </is>
       </c>
     </row>
@@ -2207,25 +2207,25 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>플라이밀 단백질쉐이크 45g 9종 택1</t>
+          <t>[8월 올영픽/트러블 1등] 파티온 노스카나인 트러블 세럼 50ml 기획(+15ml+마스크 1매)</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2,970원 ~</t>
+          <t>26,500원</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>2970</v>
+        <v>26500</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000190168&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=63</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000219717&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=63</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.709487+09:00</t>
+          <t>2025-08-13T02:53:02.275287+09:00</t>
         </is>
       </c>
     </row>
@@ -2235,25 +2235,25 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>[수분진정] 아비브 어성초 카밍 토너 스킨부스터 더블 기획 (200ml+200ml)</t>
+          <t>[올영 어워즈 1등 크림]에스트라 아토베리어365 크림 80ml</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>27,300원</t>
+          <t>33,000원</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>27300</v>
+        <v>33000</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000155253&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=64</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000198320&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=64</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.750866+09:00</t>
+          <t>2025-08-13T02:53:02.323479+09:00</t>
         </is>
       </c>
     </row>
@@ -2263,25 +2263,25 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>(50%용량증정)에스트라 더마UV365 장벽수분 무기자차 선크림 40ml+20ml 기획</t>
+          <t>[1등세럼] 브링그린 징크테카 트러블 세럼 기획 50ml 리필기획</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>24,800원</t>
+          <t>29,800원 ~</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>24800</v>
+        <v>29800</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000206826&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=65</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000228890&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=65</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.794864+09:00</t>
+          <t>2025-08-13T02:53:02.374297+09:00</t>
         </is>
       </c>
     </row>
@@ -2291,25 +2291,25 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>[8월 올영픽] 아이오페 레티놀 슈퍼 바운스 세럼 30ml 한정기획 (+20ml+선앰플 20ml)</t>
+          <t>[테리백증정]해피바스 티트리시카 등드름 케어바디워시 900G</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>38,300원</t>
+          <t>8,900원 ~</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>38300</v>
+        <v>8900</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000224685&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=66</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000202527&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=66</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.837385+09:00</t>
+          <t>2025-08-13T02:53:02.422299+09:00</t>
         </is>
       </c>
     </row>
@@ -2319,25 +2319,25 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>[테리백증정]해피바스 티트리시카 등드름 케어바디워시 900G</t>
+          <t>[8월 올영픽/이사배브랜드] 투슬래시포 엔젤릭 새틴 쿠션 기획 (+파우치 증정)</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>8,900원 ~</t>
+          <t>37,800원 ~</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>8900</v>
+        <v>37800</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000202527&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=67</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231020&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=67</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.882159+09:00</t>
+          <t>2025-08-13T02:53:02.471266+09:00</t>
         </is>
       </c>
     </row>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.936269+09:00</t>
+          <t>2025-08-13T02:53:02.521674+09:00</t>
         </is>
       </c>
     </row>
@@ -2375,25 +2375,25 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>식물나라 가벼운 수분 선 젤 60ml (단품/2개입)</t>
+          <t>[백태순삭] 라덴스 베럴 혀클리너 (블루/그레이)</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>13,800원 ~</t>
+          <t>8,460원 ~</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>13800</v>
+        <v>8460</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000223906&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=69</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000173609&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=69</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:11.970695+09:00</t>
+          <t>2025-08-13T02:53:02.582253+09:00</t>
         </is>
       </c>
     </row>
@@ -2403,25 +2403,25 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>[8월 올영픽/트러블 1등] 파티온 노스카나인 트러블 세럼 50ml 기획(+15ml+마스크 1매)</t>
+          <t>[뷰티디바이스 1위] [광채토닝 메디큐브 부스터프로 쿠로미 에디션(+쿠로미헤드캡+세안밴드+디바이스클리너+스티커2종)</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>26,500원</t>
+          <t>349,000원</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>26500</v>
+        <v>349000</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000219717&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=70</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000224654&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=70</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.007044+09:00</t>
+          <t>2025-08-13T02:53:02.626042+09:00</t>
         </is>
       </c>
     </row>
@@ -2431,25 +2431,25 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>[수분진정/세럼증정] 닥터지 레드 블레미쉬 클리어 수딩 크림 70ml 증정기획 2종</t>
+          <t>[8월 올영픽/대용량] 바이오가 등드름 바디워시 베타인살리실레이트 1000ml</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>27,600원 ~</t>
+          <t>21,160원</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>27600</v>
+        <v>21160</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000164615&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=71</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000209207&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=71</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.039074+09:00</t>
+          <t>2025-08-13T02:53:02.666519+09:00</t>
         </is>
       </c>
     </row>
@@ -2459,25 +2459,25 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>[8월 올영픽/대용량] 바이오가 등드름 바디워시 베타인살리실레이트 1000ml</t>
+          <t>[수분진정/세럼증정] 닥터지 레드 블레미쉬 클리어 수딩 크림 70ml 증정기획 2종</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>21,160원</t>
+          <t>27,600원 ~</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>21160</v>
+        <v>27600</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000209207&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=72</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000164615&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=72</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.084750+09:00</t>
+          <t>2025-08-13T02:53:02.715109+09:00</t>
         </is>
       </c>
     </row>
@@ -2487,25 +2487,25 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>[1위수상] 토리든 마스크 10매 기획 3종 (수분/진정/브라이트닝)</t>
+          <t>[3년 연속 1위] 콜레올로지 PRO 600mg*30정/60정 (15일/1개월분)</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>14,500원 ~</t>
+          <t>16,900원 ~</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>14500</v>
+        <v>16900</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000158752&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=73</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000175634&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=73</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.128915+09:00</t>
+          <t>2025-08-13T02:53:02.765834+09:00</t>
         </is>
       </c>
     </row>
@@ -2515,25 +2515,25 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>[8월 올영픽/이사배브랜드] 투슬래시포 엔젤릭 새틴 쿠션 기획 (+파우치 증정)</t>
+          <t>[8월 올영픽] [유시몰X헌터] 장화스탠더+퍼플코렉터 미백치약 106g*2</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>37,800원 ~</t>
+          <t>25,900원</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>37800</v>
+        <v>25900</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231020&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=74</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230647&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=74</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.167552+09:00</t>
+          <t>2025-08-13T02:53:02.812859+09:00</t>
         </is>
       </c>
     </row>
@@ -2543,25 +2543,25 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>[KBO 키링 랜덤 증정] 메디힐 마데카소사이드 수분 선 세럼 흔적 리페어 50g 기획(KBO 에디션)</t>
+          <t>아디다스 EDP 30ml/50ml/100ml 6종 택 1</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>13,600원 ~</t>
+          <t>20,200원 ~</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>13600</v>
+        <v>20200</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231037&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=75</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230142&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=75</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.207422+09:00</t>
+          <t>2025-08-13T02:53:02.854883+09:00</t>
         </is>
       </c>
     </row>
@@ -2571,25 +2571,25 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>페리페라 스피디 스키니 브로우 7 Colors</t>
+          <t>[8월 올영픽/포켓몬 에디션]성분에디터 실크펩타이드 EGF 하트핏 볼륨 리프팅 앰플 40ml 더블 기획(+키링 파우치)</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>5,700원 ~</t>
+          <t>25,800원</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>5700</v>
+        <v>25800</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000138671&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=76</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231076&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=76</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.248968+09:00</t>
+          <t>2025-08-13T02:53:02.893053+09:00</t>
         </is>
       </c>
     </row>
@@ -2599,25 +2599,25 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>[8월 올영픽][NEW/단독기획]하트퍼센트 도트 온 무드 립펜슬 0.8g 22종 (기획/단품)</t>
+          <t>[8월 올영픽/하트거울증정] 이니스프리 비타민C 그린티 엔자임 세럼 30ml 더블 기획</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>11,900원 ~</t>
+          <t>28,220원</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>11900</v>
+        <v>28220</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000174066&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=77</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230206&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=77</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.287924+09:00</t>
+          <t>2025-08-13T02:53:02.931808+09:00</t>
         </is>
       </c>
     </row>
@@ -2627,25 +2627,25 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>[1등세럼] 브링그린 징크테카 트러블 세럼 기획 50ml 리필기획</t>
+          <t>[8월올영픽/단독기획] 프리메라 비타티놀 바운시 리프트 세럼 30g+20g 기획</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>29,800원 ~</t>
+          <t>31,200원 ~</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>29800</v>
+        <v>31200</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000228890&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=78</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231293&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=78</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.332664+09:00</t>
+          <t>2025-08-13T02:53:02.986262+09:00</t>
         </is>
       </c>
     </row>
@@ -2655,25 +2655,25 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>[미니 속광도화밤 증정 기획] 투크 워터프루프 슬림 아이라이너 17colors (기획/단품)</t>
+          <t>헤라 블랙쿠션 본품15g+리필15g</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>11,900원 ~</t>
+          <t>66,600원 ~</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>11900</v>
+        <v>66600</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000185046&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=79</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000202777&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=79</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.367748+09:00</t>
+          <t>2025-08-13T02:53:03.041211+09:00</t>
         </is>
       </c>
     </row>
@@ -2683,25 +2683,25 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>[올영 어워즈 1등 크림]에스트라 아토베리어365 크림 80ml</t>
+          <t>[8월 올영픽][NEW/단독기획]하트퍼센트 도트 온 무드 립펜슬 0.8g 22종 (기획/단품)</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>33,000원</t>
+          <t>11,900원 ~</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>33000</v>
+        <v>11900</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000198320&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=80</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000174066&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=80</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.408402+09:00</t>
+          <t>2025-08-13T02:53:03.083925+09:00</t>
         </is>
       </c>
     </row>
@@ -2711,25 +2711,25 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>[3년 연속 1위] 콜레올로지 PRO 600mg*30정/60정 (15일/1개월분)</t>
+          <t>웨이크메이크 소프트 블러링 아이팔레트 25COLOR(단품/기획)</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>16,900원 ~</t>
+          <t>23,800원 ~</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>16900</v>
+        <v>23800</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000175634&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=81</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000180532&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=81</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.452556+09:00</t>
+          <t>2025-08-13T02:53:03.128336+09:00</t>
         </is>
       </c>
     </row>
@@ -2739,25 +2739,25 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>[백태순삭] 라덴스 베럴 혀클리너 (블루/그레이)</t>
+          <t>[진정커버/1위쿠션] 파넬 시카마누 세럼쿠션(본품+리필)</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>8,460원 ~</t>
+          <t>27,750원 ~</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>8460</v>
+        <v>27750</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000173609&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=82</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000190611&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=82</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.494718+09:00</t>
+          <t>2025-08-13T02:53:03.177919+09:00</t>
         </is>
       </c>
     </row>
@@ -2767,25 +2767,25 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>[8/12 하루특가[Y존냄새제거] 바솔 포밍워시 여성청결제 기획(이너밸런싱/마일드캄) 4종 택 1</t>
+          <t>(50%용량증정)에스트라 더마UV365 장벽수분 무기자차 선크림 40ml+20ml 기획</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>17,200원 ~</t>
+          <t>24,800원</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>17200</v>
+        <v>24800</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000204867&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=83</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000206826&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=83</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.544091+09:00</t>
+          <t>2025-08-13T02:53:03.236603+09:00</t>
         </is>
       </c>
     </row>
@@ -2795,25 +2795,25 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>헤라 블랙쿠션 본품15g+리필15g</t>
+          <t>페리페라 스피디 스키니 브로우 7 Colors</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>66,600원 ~</t>
+          <t>5,700원 ~</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>66600</v>
+        <v>5700</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000202777&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=84</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000138671&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=84</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.589019+09:00</t>
+          <t>2025-08-13T02:53:03.293371+09:00</t>
         </is>
       </c>
     </row>
@@ -2823,25 +2823,25 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>웨이크메이크 소프트 블러링 아이팔레트 25COLOR(단품/기획)</t>
+          <t>[KBO 키링 랜덤 증정] 메디힐 마데카소사이드 수분 선 세럼 흔적 리페어 50g 기획(KBO 에디션)</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>23,800원 ~</t>
+          <t>13,600원 ~</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>23800</v>
+        <v>13600</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000180532&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=85</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231037&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=85</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.643773+09:00</t>
+          <t>2025-08-13T02:53:03.350116+09:00</t>
         </is>
       </c>
     </row>
@@ -2851,25 +2851,25 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>[증정기획/대용량] 토리든 다이브인 저분자 히알루론산 토너 500ml 기획 (+화장솜 60매 증정)</t>
+          <t>[미니 속광도화밤 증정 기획] 투크 워터프루프 슬림 아이라이너 17colors (기획/단품)</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>21,750원</t>
+          <t>11,900원 ~</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>21750</v>
+        <v>11900</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000180474&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=86</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000185046&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=86</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.691832+09:00</t>
+          <t>2025-08-13T02:53:03.403999+09:00</t>
         </is>
       </c>
     </row>
@@ -2879,25 +2879,25 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>[흔적진정] 마몽드 카밍 샷 아줄렌 흔적 수분 앰플 50ml 기획</t>
+          <t>[8/12 하루특가[Y존냄새제거] 바솔 포밍워시 여성청결제 기획(이너밸런싱/마일드캄) 4종 택 1</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>18,900원 ~</t>
+          <t>17,200원 ~</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>18900</v>
+        <v>17200</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000219389&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=87</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000204867&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=87</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.737151+09:00</t>
+          <t>2025-08-13T02:53:03.453722+09:00</t>
         </is>
       </c>
     </row>
@@ -2907,25 +2907,25 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>[8월올영픽/미니틴트증정] 라카 맥시 글레이어 틴트 3.8g 20종 (단품/기획)</t>
+          <t>[말끔모공/피지순삭] 아누아 어성초 클렌징 듀오 기획 (오일 200ml+폼 150ml)</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>13,500원 ~</t>
+          <t>25,500원</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>13500</v>
+        <v>25500</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000228370&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=88</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000225774&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=88</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.779863+09:00</t>
+          <t>2025-08-13T02:53:03.496832+09:00</t>
         </is>
       </c>
     </row>
@@ -2935,25 +2935,25 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>[8월올영픽/단독기획] 프리메라 비타티놀 바운시 리프트 세럼 30g+20g 기획</t>
+          <t>[단독/추가증정] 1+1 려 루트젠 탈모증상케어 두피에센스 80ml 더블기획+샴푸50ml</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>31,200원 ~</t>
+          <t>21,900원 ~</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>31200</v>
+        <v>21900</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231293&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=89</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000197603&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=89</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.828665+09:00</t>
+          <t>2025-08-13T02:53:03.547653+09:00</t>
         </is>
       </c>
     </row>
@@ -2963,25 +2963,25 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>[8월 올영픽/하트거울증정] 이니스프리 비타민C 그린티 엔자임 세럼 30ml 더블 기획</t>
+          <t>[8월올영픽/미니틴트증정] 라카 맥시 글레이어 틴트 3.8g 20종 (단품/기획)</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>28,220원</t>
+          <t>13,500원 ~</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>28220</v>
+        <v>13500</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230206&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=90</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000228370&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=90</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.856311+09:00</t>
+          <t>2025-08-13T02:53:03.598244+09:00</t>
         </is>
       </c>
     </row>
@@ -2991,25 +2991,25 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>[진정커버/1위쿠션] 파넬 시카마누 세럼쿠션(본품+리필)</t>
+          <t>[흔적진정] 마몽드 카밍 샷 아줄렌 흔적 수분 앰플 50ml 기획</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>27,750원 ~</t>
+          <t>18,900원 ~</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>27750</v>
+        <v>18900</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000190611&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=91</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000219389&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=91</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.906299+09:00</t>
+          <t>2025-08-13T02:53:03.649185+09:00</t>
         </is>
       </c>
     </row>
@@ -3019,25 +3019,25 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>[말끔모공/피지순삭] 아누아 어성초 클렌징 듀오 기획 (오일 200ml+폼 150ml)</t>
+          <t>[백태순삭] 라덴스 베럴 혀클리너 (블루/블랙/그레이/화이트)</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>25,500원</t>
+          <t>8,460원 ~</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>25500</v>
+        <v>8460</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000225774&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=92</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000159233&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=92</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.946550+09:00</t>
+          <t>2025-08-13T02:53:03.693045+09:00</t>
         </is>
       </c>
     </row>
@@ -3047,25 +3047,25 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>[8월 올영픽/포켓몬 에디션]성분에디터 실크펩타이드 EGF 하트핏 볼륨 리프팅 앰플 40ml 더블 기획(+키링 파우치)</t>
+          <t>[8월 올영픽] 오프온 등드름 바디워시(+천연 루파스펀지 증정)</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>25,800원</t>
+          <t>22,300원 ~</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>25800</v>
+        <v>22300</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000231076&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=93</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000211096&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=93</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:12.989758+09:00</t>
+          <t>2025-08-13T02:53:03.739746+09:00</t>
         </is>
       </c>
     </row>
@@ -3075,25 +3075,25 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>[백태순삭] 라덴스 베럴 혀클리너 (블루/블랙/그레이/화이트)</t>
+          <t>딜라이트 프로젝트 헬시간식 모음전 (쉐이크/음료/프로틴스낵)</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>8,460원 ~</t>
+          <t>2,800원 ~</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>8460</v>
+        <v>2800</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000159233&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=94</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000216127&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=94</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:13.041987+09:00</t>
+          <t>2025-08-13T02:53:03.790783+09:00</t>
         </is>
       </c>
     </row>
@@ -3103,25 +3103,25 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>[8월 올영픽] 구달 청귤 비타C 잡티케어 크림 알파 75ml 리필 기획</t>
+          <t>바세린 컬러 + 케어 립밤 4.2g 더블 기획 2종 (+빗 키링 증정)</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>22,300원</t>
+          <t>8,780원 ~</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>22300</v>
+        <v>8780</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230655&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=95</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000227013&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=95</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:13.099610+09:00</t>
+          <t>2025-08-13T02:53:03.844157+09:00</t>
         </is>
       </c>
     </row>
@@ -3131,25 +3131,25 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>아디다스 EDP 30ml/50ml/100ml 6종 택 1</t>
+          <t>[증정기획/대용량] 토리든 다이브인 저분자 히알루론산 토너 500ml 기획 (+화장솜 60매 증정)</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>20,200원 ~</t>
+          <t>21,750원</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>20200</v>
+        <v>21750</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000230142&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=96</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000180474&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=96</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:13.137742+09:00</t>
+          <t>2025-08-13T02:53:03.893214+09:00</t>
         </is>
       </c>
     </row>
@@ -3177,7 +3177,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:13.165880+09:00</t>
+          <t>2025-08-13T02:53:03.946471+09:00</t>
         </is>
       </c>
     </row>
@@ -3187,25 +3187,25 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>[8월 올영픽/핑구콜라보] 코스노리 아이래쉬 틴팅 세럼 비건 블랙 속눈썹영양제 (단품/기획)</t>
+          <t>아누아 비타민씨 잡티 세럼 마스크 10매입</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>14,400원 ~</t>
+          <t>15,000원</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>14400</v>
+        <v>15000</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000187890&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=98</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000222734&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=98</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:13.190319+09:00</t>
+          <t>2025-08-13T02:53:03.996333+09:00</t>
         </is>
       </c>
     </row>
@@ -3215,25 +3215,25 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>[단독/추가증정] 1+1 려 루트젠 탈모증상케어 두피에센스 80ml 더블기획+샴푸50ml</t>
+          <t>[화잘먹] 구달 맑은 어성초 진정 수분 선크림 50ml 1+1 기획</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>21,900원 ~</t>
+          <t>16,500원 ~</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>21900</v>
+        <v>16500</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000197603&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=99</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000219553&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=99</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:13.224008+09:00</t>
+          <t>2025-08-13T02:53:04.046853+09:00</t>
         </is>
       </c>
     </row>
@@ -3243,25 +3243,25 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>[화잘먹] 구달 맑은 어성초 진정 수분 선크림 50ml 1+1 기획</t>
+          <t>[550만판매/1등피지클리너]일소 슈퍼 멜팅 세범 소프트너 150ml 기획 (+착붙솜 40매+모공 텐션 마스크팩 1매</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>16,500원 ~</t>
+          <t>17,900원</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>16500</v>
+        <v>17900</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000219553&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=100</t>
+          <t>https://www.oliveyoung.co.kr/store/goods/getGoodsDetail.do?goodsNo=A000000225736&amp;dispCatNo=90000010009&amp;trackingCd=Best_Sellingbest&amp;t_page=랭킹&amp;t_click=판매랭킹_전체_상품상세&amp;t_number=100</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>2025-08-13T02:16:13.255780+09:00</t>
+          <t>2025-08-13T02:53:04.112153+09:00</t>
         </is>
       </c>
     </row>

</xml_diff>